<commit_message>
Error handler for registering a new parent.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
   <si>
     <t>Number</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Authentification</t>
   </si>
   <si>
-    <t>Login Failed.</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Account is already exist.</t>
   </si>
   <si>
-    <t>The note has been updated successfully.</t>
-  </si>
-  <si>
     <t>http://dev.mysql.com/doc/refman/5.5/en/error-messages-server.html</t>
   </si>
   <si>
@@ -221,16 +215,34 @@
     <t>Network disconnected.</t>
   </si>
   <si>
-    <t>The note has been created successfully.</t>
-  </si>
-  <si>
     <t>Response</t>
   </si>
   <si>
     <t>Press the button to delete this note.</t>
   </si>
   <si>
-    <t>The note has been deleted successfully.</t>
+    <t>Not a valid e-mail address.</t>
+  </si>
+  <si>
+    <t>New parent has been registered.</t>
+  </si>
+  <si>
+    <t>The note has been created.</t>
+  </si>
+  <si>
+    <t>The note has been updated.</t>
+  </si>
+  <si>
+    <t>The note has been deleted.</t>
+  </si>
+  <si>
+    <t>Access is not authorized.</t>
+  </si>
+  <si>
+    <t>Failed to log in.</t>
+  </si>
+  <si>
+    <t>Not an admin account.</t>
   </si>
 </sst>
 </file>
@@ -583,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,12 +611,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -621,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -632,10 +644,10 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -643,13 +655,13 @@
         <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -657,13 +669,13 @@
         <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -671,13 +683,13 @@
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,13 +697,13 @@
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -733,7 +745,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -747,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -761,7 +773,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -775,7 +787,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -789,7 +801,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -803,7 +815,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -817,7 +829,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,7 +857,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,7 +871,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -887,7 +899,7 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -901,7 +913,7 @@
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,7 +927,7 @@
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,7 +941,7 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -943,7 +955,7 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -957,7 +969,7 @@
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,7 +983,7 @@
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -985,7 +997,7 @@
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -999,7 +1011,7 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1013,7 +1025,7 @@
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1027,7 +1039,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1041,7 +1053,7 @@
         <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1055,7 +1067,7 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1069,7 +1081,7 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1083,7 +1095,7 @@
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,7 +1109,7 @@
         <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,7 +1123,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,7 +1137,7 @@
         <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,7 +1151,7 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1153,7 +1165,7 @@
         <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,7 +1179,7 @@
         <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,7 +1193,7 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1195,7 +1207,7 @@
         <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,7 +1221,7 @@
         <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,7 +1235,7 @@
         <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,7 +1249,7 @@
         <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,7 +1263,7 @@
         <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,13 +1271,13 @@
         <v>602</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,13 +1285,13 @@
         <v>603</v>
       </c>
       <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
         <v>47</v>
       </c>
-      <c r="C49" t="s">
-        <v>48</v>
-      </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,13 +1299,13 @@
         <v>604</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,13 +1313,13 @@
         <v>605</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D51" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,10 +1327,10 @@
         <v>606</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
         <v>2</v>
@@ -1326,77 +1338,133 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>901</v>
+        <v>607</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B54" t="s">
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B55" t="s">
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D55" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>55</v>
+      <c r="A56">
+        <v>902</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>607</v>
+        <v>903</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>904</v>
+      </c>
+      <c r="B58" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+      <c r="D58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>905</v>
+      </c>
+      <c r="B59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
         <v>65</v>
+      </c>
+      <c r="D59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>906</v>
+      </c>
+      <c r="B60" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2">
-    <sortState ref="A3:D56">
+    <sortState ref="A3:D61">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Add error handler for updating tree info.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
   <si>
     <t>Number</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Not an admin account.</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>The tree has been updated.</t>
   </si>
 </sst>
 </file>
@@ -309,11 +315,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,11 +616,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
       <c r="H1" t="s">
         <v>51</v>
       </c>
@@ -632,7 +638,7 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -707,7 +713,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1459,6 +1465,20 @@
         <v>55</v>
       </c>
       <c r="D61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>634</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix "delete tree" feature.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="79">
   <si>
     <t>Number</t>
   </si>
@@ -227,9 +227,6 @@
     <t>New parent has been registered.</t>
   </si>
   <si>
-    <t>The note has been created.</t>
-  </si>
-  <si>
     <t>The note has been updated.</t>
   </si>
   <si>
@@ -249,6 +246,24 @@
   </si>
   <si>
     <t>The tree has been updated.</t>
+  </si>
+  <si>
+    <t>The tree has been adopted.</t>
+  </si>
+  <si>
+    <t>The tree has ben unadopted.</t>
+  </si>
+  <si>
+    <t>New tree has been created.</t>
+  </si>
+  <si>
+    <t>New note has been posted.</t>
+  </si>
+  <si>
+    <t>Press the button to delete this tree.</t>
+  </si>
+  <si>
+    <t>The tree has been deleted.</t>
   </si>
 </sst>
 </file>
@@ -601,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1323,7 @@
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" t="s">
         <v>62</v>
@@ -1322,7 +1337,7 @@
         <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D51" t="s">
         <v>62</v>
@@ -1350,7 +1365,7 @@
         <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D53" t="s">
         <v>62</v>
@@ -1358,13 +1373,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>900</v>
+        <v>634</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D54" t="s">
         <v>62</v>
@@ -1372,13 +1387,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>901</v>
+        <v>635</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D55" t="s">
         <v>62</v>
@@ -1386,27 +1401,27 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>902</v>
+        <v>636</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>903</v>
+        <v>638</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="D57" t="s">
         <v>62</v>
@@ -1414,13 +1429,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>904</v>
+        <v>639</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D58" t="s">
         <v>62</v>
@@ -1428,13 +1443,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="B59" t="s">
         <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D59" t="s">
         <v>62</v>
@@ -1442,27 +1457,27 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="B60" t="s">
         <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>53</v>
+      <c r="A61">
+        <v>902</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D61" t="s">
         <v>62</v>
@@ -1470,21 +1485,91 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>634</v>
+        <v>903</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>904</v>
+      </c>
+      <c r="B63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>905</v>
+      </c>
+      <c r="B64" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>906</v>
+      </c>
+      <c r="B65" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>637</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2">
-    <sortState ref="A3:D61">
+    <sortState ref="A3:D66">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Base donation map setup & control panel.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
   <si>
     <t>Number</t>
   </si>
@@ -264,6 +264,21 @@
   </si>
   <si>
     <t>The tree has been deleted.</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>The location has been updated.</t>
+  </si>
+  <si>
+    <t>New location has been created.</t>
+  </si>
+  <si>
+    <t>The location has been deleted.</t>
+  </si>
+  <si>
+    <t>Press the button to delete this location.</t>
   </si>
 </sst>
 </file>
@@ -616,21 +631,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -640,7 +655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -657,7 +672,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -671,7 +686,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>90</v>
       </c>
@@ -685,7 +700,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>91</v>
       </c>
@@ -699,7 +714,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>92</v>
       </c>
@@ -713,7 +728,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>93</v>
       </c>
@@ -727,7 +742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>100</v>
       </c>
@@ -741,7 +756,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>101</v>
       </c>
@@ -755,7 +770,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>200</v>
       </c>
@@ -769,7 +784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>201</v>
       </c>
@@ -783,7 +798,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>202</v>
       </c>
@@ -797,7 +812,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>203</v>
       </c>
@@ -811,7 +826,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>204</v>
       </c>
@@ -825,7 +840,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>205</v>
       </c>
@@ -839,7 +854,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>206</v>
       </c>
@@ -853,7 +868,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>300</v>
       </c>
@@ -867,7 +882,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>301</v>
       </c>
@@ -881,7 +896,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>302</v>
       </c>
@@ -895,7 +910,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>303</v>
       </c>
@@ -909,7 +924,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>304</v>
       </c>
@@ -923,7 +938,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>305</v>
       </c>
@@ -937,7 +952,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>307</v>
       </c>
@@ -951,7 +966,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>400</v>
       </c>
@@ -965,7 +980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>401</v>
       </c>
@@ -979,7 +994,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>402</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>403</v>
       </c>
@@ -1007,7 +1022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>404</v>
       </c>
@@ -1021,7 +1036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>405</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>406</v>
       </c>
@@ -1049,7 +1064,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>407</v>
       </c>
@@ -1063,7 +1078,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>408</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>409</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>410</v>
       </c>
@@ -1105,7 +1120,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>411</v>
       </c>
@@ -1119,7 +1134,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>412</v>
       </c>
@@ -1133,7 +1148,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>413</v>
       </c>
@@ -1147,7 +1162,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>414</v>
       </c>
@@ -1161,7 +1176,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>415</v>
       </c>
@@ -1175,7 +1190,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>416</v>
       </c>
@@ -1189,7 +1204,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>417</v>
       </c>
@@ -1203,7 +1218,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>500</v>
       </c>
@@ -1217,7 +1232,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>501</v>
       </c>
@@ -1231,7 +1246,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>502</v>
       </c>
@@ -1245,7 +1260,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>503</v>
       </c>
@@ -1259,7 +1274,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>504</v>
       </c>
@@ -1273,7 +1288,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>505</v>
       </c>
@@ -1287,7 +1302,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>602</v>
       </c>
@@ -1301,7 +1316,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>603</v>
       </c>
@@ -1315,7 +1330,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>604</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>605</v>
       </c>
@@ -1343,7 +1358,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>606</v>
       </c>
@@ -1357,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>607</v>
       </c>
@@ -1371,7 +1386,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>634</v>
       </c>
@@ -1385,7 +1400,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>635</v>
       </c>
@@ -1399,7 +1414,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>636</v>
       </c>
@@ -1413,163 +1428,219 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B57" t="s">
         <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B58" t="s">
         <v>71</v>
       </c>
       <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>639</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
         <v>74</v>
       </c>
-      <c r="D58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="D59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>664</v>
+      </c>
+      <c r="B60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>665</v>
+      </c>
+      <c r="B61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>666</v>
+      </c>
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>667</v>
+      </c>
+      <c r="B63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>900</v>
-      </c>
-      <c r="B59" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>901</v>
-      </c>
-      <c r="B60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" t="s">
-        <v>68</v>
-      </c>
-      <c r="D60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>902</v>
-      </c>
-      <c r="B61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>903</v>
-      </c>
-      <c r="B62" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>904</v>
-      </c>
-      <c r="B63" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>905</v>
       </c>
       <c r="B64" t="s">
         <v>45</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="B65" t="s">
         <v>45</v>
       </c>
       <c r="C65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>902</v>
+      </c>
+      <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>903</v>
+      </c>
+      <c r="B67" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>904</v>
+      </c>
+      <c r="B68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" t="s">
+        <v>64</v>
+      </c>
+      <c r="D68" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>905</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>906</v>
+      </c>
+      <c r="B70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" t="s">
         <v>70</v>
       </c>
-      <c r="D65" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>53</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B71" t="s">
         <v>54</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C71" t="s">
         <v>55</v>
       </c>
-      <c r="D66" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>637</v>
-      </c>
-      <c r="B67" t="s">
-        <v>71</v>
-      </c>
-      <c r="C67" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="D71" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2">
-    <sortState ref="A3:D66">
+    <sortState ref="A3:D71">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Adding a new donation panel.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -633,19 +633,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:D63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -655,7 +655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -686,7 +686,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>90</v>
       </c>
@@ -700,7 +700,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>91</v>
       </c>
@@ -714,7 +714,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>92</v>
       </c>
@@ -728,7 +728,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>93</v>
       </c>
@@ -742,7 +742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>100</v>
       </c>
@@ -756,7 +756,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>101</v>
       </c>
@@ -770,7 +770,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>200</v>
       </c>
@@ -784,7 +784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>201</v>
       </c>
@@ -798,7 +798,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>202</v>
       </c>
@@ -812,7 +812,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>203</v>
       </c>
@@ -826,7 +826,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>204</v>
       </c>
@@ -840,7 +840,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>205</v>
       </c>
@@ -854,7 +854,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>206</v>
       </c>
@@ -868,7 +868,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>300</v>
       </c>
@@ -882,7 +882,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>301</v>
       </c>
@@ -896,7 +896,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>302</v>
       </c>
@@ -910,7 +910,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>303</v>
       </c>
@@ -924,7 +924,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>304</v>
       </c>
@@ -938,7 +938,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>305</v>
       </c>
@@ -952,7 +952,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>307</v>
       </c>
@@ -966,7 +966,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>400</v>
       </c>
@@ -980,7 +980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>401</v>
       </c>
@@ -994,7 +994,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>402</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>403</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>404</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>405</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>406</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>407</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>408</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>409</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>410</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>411</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>412</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>413</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>414</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>415</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>416</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>417</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>500</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>501</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>502</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>503</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>504</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>505</v>
       </c>
@@ -1302,12 +1302,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>602</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
         <v>48</v>
@@ -1316,12 +1316,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>603</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
         <v>47</v>
@@ -1330,7 +1330,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>604</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>605</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>606</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>607</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>634</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>635</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>636</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>637</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>638</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>639</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>664</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>665</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>666</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>667</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>900</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>901</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>902</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>903</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>904</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>905</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>906</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Finish "add/delete/edit location" feature.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="86">
   <si>
     <t>Number</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>Press the button to delete this location.</t>
+  </si>
+  <si>
+    <t>Donate</t>
+  </si>
+  <si>
+    <t>Press the button to delete this donation.</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,6 +1642,20 @@
       </c>
       <c r="D71" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>706</v>
+      </c>
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "Unable / Enable Adopting" feature.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="186">
   <si>
     <t>Number</t>
   </si>
@@ -576,6 +576,15 @@
   </si>
   <si>
     <t>NEW PLACE</t>
+  </si>
+  <si>
+    <t>Currently unable to adopt</t>
+  </si>
+  <si>
+    <t>Currnetly Adoptable  (Click to change)</t>
+  </si>
+  <si>
+    <t>Currnetly Unadoptable  (Click to change)</t>
   </si>
 </sst>
 </file>
@@ -928,21 +937,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H168"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -952,7 +961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -969,7 +978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -983,7 +992,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>90</v>
       </c>
@@ -997,7 +1006,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>91</v>
       </c>
@@ -1011,7 +1020,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>92</v>
       </c>
@@ -1025,7 +1034,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>93</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>100</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>101</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>200</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>201</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>202</v>
       </c>
@@ -1109,7 +1118,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>203</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>204</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>205</v>
       </c>
@@ -1151,7 +1160,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>206</v>
       </c>
@@ -1165,7 +1174,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>300</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>301</v>
       </c>
@@ -1193,7 +1202,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>302</v>
       </c>
@@ -1207,7 +1216,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>303</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>304</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>305</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>307</v>
       </c>
@@ -1263,7 +1272,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>400</v>
       </c>
@@ -1277,7 +1286,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>401</v>
       </c>
@@ -1291,7 +1300,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>402</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>403</v>
       </c>
@@ -1319,7 +1328,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>404</v>
       </c>
@@ -1333,7 +1342,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>405</v>
       </c>
@@ -1347,7 +1356,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>406</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>407</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>408</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>409</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>410</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>411</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>412</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>413</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>414</v>
       </c>
@@ -1473,7 +1482,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>415</v>
       </c>
@@ -1487,7 +1496,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>416</v>
       </c>
@@ -1501,7 +1510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>417</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>500</v>
       </c>
@@ -1529,7 +1538,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>501</v>
       </c>
@@ -1543,7 +1552,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>502</v>
       </c>
@@ -1557,7 +1566,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>503</v>
       </c>
@@ -1571,7 +1580,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>504</v>
       </c>
@@ -1585,7 +1594,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>505</v>
       </c>
@@ -1599,7 +1608,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>601</v>
       </c>
@@ -1613,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>602</v>
       </c>
@@ -1627,7 +1636,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>603</v>
       </c>
@@ -1641,7 +1650,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>604</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>605</v>
       </c>
@@ -1669,7 +1678,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>606</v>
       </c>
@@ -1683,7 +1692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>607</v>
       </c>
@@ -1697,7 +1706,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>608</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>609</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>610</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>611</v>
       </c>
@@ -1753,7 +1762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>612</v>
       </c>
@@ -1767,7 +1776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>613</v>
       </c>
@@ -1781,7 +1790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>627</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>628</v>
       </c>
@@ -1809,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>629</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>630</v>
       </c>
@@ -1837,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>631</v>
       </c>
@@ -1851,7 +1860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>632</v>
       </c>
@@ -1865,7 +1874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>633</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>634</v>
       </c>
@@ -1893,7 +1902,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>635</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>636</v>
       </c>
@@ -1921,7 +1930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>637</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>638</v>
       </c>
@@ -1949,7 +1958,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>639</v>
       </c>
@@ -1963,7 +1972,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>640</v>
       </c>
@@ -1977,7 +1986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>641</v>
       </c>
@@ -1991,7 +2000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>662</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>663</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>664</v>
       </c>
@@ -2033,7 +2042,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>665</v>
       </c>
@@ -2047,7 +2056,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>666</v>
       </c>
@@ -2061,7 +2070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>667</v>
       </c>
@@ -2075,7 +2084,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>668</v>
       </c>
@@ -2089,7 +2098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>669</v>
       </c>
@@ -2103,7 +2112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>670</v>
       </c>
@@ -2117,7 +2126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>671</v>
       </c>
@@ -2131,7 +2140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>672</v>
       </c>
@@ -2145,7 +2154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>673</v>
       </c>
@@ -2159,1125 +2168,1167 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
+        <v>676</v>
+      </c>
+      <c r="B88" t="s">
+        <v>108</v>
+      </c>
+      <c r="C88" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>677</v>
+      </c>
+      <c r="B89" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" t="s">
+        <v>166</v>
+      </c>
+      <c r="D89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>678</v>
+      </c>
+      <c r="B90" t="s">
+        <v>108</v>
+      </c>
+      <c r="C90" t="s">
+        <v>167</v>
+      </c>
+      <c r="D90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>679</v>
+      </c>
+      <c r="B91" t="s">
+        <v>108</v>
+      </c>
+      <c r="C91" t="s">
+        <v>168</v>
+      </c>
+      <c r="D91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>680</v>
+      </c>
+      <c r="B92" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" t="s">
+        <v>169</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>681</v>
+      </c>
+      <c r="B93" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93" t="s">
+        <v>170</v>
+      </c>
+      <c r="D93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>682</v>
+      </c>
+      <c r="B94" t="s">
+        <v>56</v>
+      </c>
+      <c r="C94" t="s">
+        <v>171</v>
+      </c>
+      <c r="D94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>683</v>
+      </c>
+      <c r="B95" t="s">
+        <v>108</v>
+      </c>
+      <c r="C95" t="s">
+        <v>172</v>
+      </c>
+      <c r="D95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>684</v>
+      </c>
+      <c r="B96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C96" t="s">
+        <v>173</v>
+      </c>
+      <c r="D96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>685</v>
+      </c>
+      <c r="B97" t="s">
+        <v>108</v>
+      </c>
+      <c r="C97" t="s">
+        <v>174</v>
+      </c>
+      <c r="D97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>686</v>
+      </c>
+      <c r="B98" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98" t="s">
+        <v>175</v>
+      </c>
+      <c r="D98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>687</v>
+      </c>
+      <c r="B99" t="s">
+        <v>108</v>
+      </c>
+      <c r="C99" t="s">
+        <v>176</v>
+      </c>
+      <c r="D99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>688</v>
+      </c>
+      <c r="B100" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100" t="s">
+        <v>177</v>
+      </c>
+      <c r="D100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>689</v>
+      </c>
+      <c r="B101" t="s">
+        <v>108</v>
+      </c>
+      <c r="C101" t="s">
+        <v>178</v>
+      </c>
+      <c r="D101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>690</v>
+      </c>
+      <c r="B102" t="s">
+        <v>108</v>
+      </c>
+      <c r="C102" t="s">
+        <v>179</v>
+      </c>
+      <c r="D102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>691</v>
+      </c>
+      <c r="B103" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" t="s">
+        <v>180</v>
+      </c>
+      <c r="D103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>692</v>
+      </c>
+      <c r="B104" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>693</v>
+      </c>
+      <c r="B105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106">
         <v>706</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B106" t="s">
         <v>84</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C106" t="s">
         <v>85</v>
       </c>
-      <c r="D88" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="D106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107">
         <v>730</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B107" t="s">
         <v>86</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C107" t="s">
         <v>87</v>
       </c>
-      <c r="D89" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="D107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108">
         <v>900</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B108" t="s">
         <v>45</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C108" t="s">
         <v>3</v>
       </c>
-      <c r="D90" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
+      <c r="D108" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109">
         <v>901</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B109" t="s">
         <v>45</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C109" t="s">
         <v>68</v>
       </c>
-      <c r="D91" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
+      <c r="D109" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110">
         <v>902</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B110" t="s">
         <v>45</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C110" t="s">
         <v>69</v>
       </c>
-      <c r="D92" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="D110" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111">
         <v>903</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B111" t="s">
         <v>45</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C111" t="s">
         <v>49</v>
       </c>
-      <c r="D93" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
+      <c r="D111" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112">
         <v>904</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B112" t="s">
         <v>45</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C112" t="s">
         <v>64</v>
       </c>
-      <c r="D94" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
+      <c r="D112" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113">
         <v>905</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B113" t="s">
         <v>45</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C113" t="s">
         <v>65</v>
       </c>
-      <c r="D95" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="D113" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114">
         <v>906</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B114" t="s">
         <v>45</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C114" t="s">
         <v>70</v>
       </c>
-      <c r="D96" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="D114" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115">
         <v>929</v>
       </c>
-      <c r="B97" t="s">
-        <v>56</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="B115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C115" t="s">
         <v>139</v>
       </c>
-      <c r="D97" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
+      <c r="D115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116">
         <v>930</v>
       </c>
-      <c r="B98" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B116" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" t="s">
         <v>138</v>
       </c>
-      <c r="D98" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
+      <c r="D116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117">
         <v>931</v>
       </c>
-      <c r="B99" t="s">
-        <v>56</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B117" t="s">
+        <v>56</v>
+      </c>
+      <c r="C117" t="s">
         <v>135</v>
       </c>
-      <c r="D99" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="D117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118">
         <v>932</v>
       </c>
-      <c r="B100" t="s">
-        <v>56</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B118" t="s">
+        <v>56</v>
+      </c>
+      <c r="C118" t="s">
         <v>134</v>
       </c>
-      <c r="D100" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
+      <c r="D118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119">
         <v>933</v>
       </c>
-      <c r="B101" t="s">
-        <v>56</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B119" t="s">
+        <v>56</v>
+      </c>
+      <c r="C119" t="s">
         <v>133</v>
       </c>
-      <c r="D101" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102">
+      <c r="D119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120">
         <v>934</v>
       </c>
-      <c r="B102" t="s">
-        <v>56</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="B120" t="s">
+        <v>56</v>
+      </c>
+      <c r="C120" t="s">
         <v>132</v>
       </c>
-      <c r="D102" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="D120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121">
         <v>935</v>
       </c>
-      <c r="B103" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="B121" t="s">
+        <v>56</v>
+      </c>
+      <c r="C121" t="s">
         <v>131</v>
       </c>
-      <c r="D103" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104">
+      <c r="D121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122">
         <v>936</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B122" t="s">
         <v>88</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C122" t="s">
         <v>89</v>
       </c>
-      <c r="D104" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="D122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123">
         <v>937</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B123" t="s">
         <v>88</v>
       </c>
-      <c r="D105" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106">
+      <c r="D123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124">
         <v>938</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B124" t="s">
         <v>88</v>
       </c>
-      <c r="D106" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107">
+      <c r="D124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125">
         <v>939</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B125" t="s">
         <v>88</v>
       </c>
-      <c r="D107" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108">
+      <c r="D125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126">
         <v>940</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B126" t="s">
         <v>88</v>
       </c>
-      <c r="D108" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109">
+      <c r="D126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127">
         <v>941</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B127" t="s">
         <v>88</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C127" t="s">
         <v>90</v>
       </c>
-      <c r="D109" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110">
+      <c r="D127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128">
         <v>960</v>
       </c>
-      <c r="B110" t="s">
-        <v>56</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="B128" t="s">
+        <v>56</v>
+      </c>
+      <c r="C128" t="s">
         <v>157</v>
       </c>
-      <c r="D110" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111">
+      <c r="D128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
         <v>961</v>
       </c>
-      <c r="B111" t="s">
-        <v>56</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="B129" t="s">
+        <v>56</v>
+      </c>
+      <c r="C129" t="s">
         <v>156</v>
       </c>
-      <c r="D111" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112">
+      <c r="D129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130">
         <v>962</v>
       </c>
-      <c r="B112" t="s">
-        <v>56</v>
-      </c>
-      <c r="C112" t="s">
+      <c r="B130" t="s">
+        <v>56</v>
+      </c>
+      <c r="C130" t="s">
         <v>91</v>
       </c>
-      <c r="D112" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113">
+      <c r="D130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131">
         <v>963</v>
       </c>
-      <c r="B113" t="s">
-        <v>56</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="B131" t="s">
+        <v>56</v>
+      </c>
+      <c r="C131" t="s">
         <v>92</v>
       </c>
-      <c r="D113" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114">
+      <c r="D131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132">
         <v>964</v>
       </c>
-      <c r="B114" t="s">
-        <v>56</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="B132" t="s">
+        <v>56</v>
+      </c>
+      <c r="C132" t="s">
         <v>93</v>
       </c>
-      <c r="D114" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115">
+      <c r="D132" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133">
         <v>965</v>
       </c>
-      <c r="B115" t="s">
-        <v>56</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="B133" t="s">
+        <v>56</v>
+      </c>
+      <c r="C133" t="s">
         <v>142</v>
       </c>
-      <c r="D115" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116">
+      <c r="D133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134">
         <v>966</v>
       </c>
-      <c r="B116" t="s">
-        <v>56</v>
-      </c>
-      <c r="C116" t="s">
+      <c r="B134" t="s">
+        <v>56</v>
+      </c>
+      <c r="C134" t="s">
         <v>143</v>
       </c>
-      <c r="D116" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117">
+      <c r="D134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135">
         <v>967</v>
       </c>
-      <c r="B117" t="s">
-        <v>56</v>
-      </c>
-      <c r="C117" t="s">
+      <c r="B135" t="s">
+        <v>56</v>
+      </c>
+      <c r="C135" t="s">
         <v>94</v>
       </c>
-      <c r="D117" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118">
+      <c r="D135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136">
         <v>968</v>
       </c>
-      <c r="B118" t="s">
-        <v>56</v>
-      </c>
-      <c r="C118" t="s">
+      <c r="B136" t="s">
+        <v>56</v>
+      </c>
+      <c r="C136" t="s">
         <v>95</v>
       </c>
-      <c r="D118" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119">
+      <c r="D136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137">
         <v>969</v>
       </c>
-      <c r="B119" t="s">
-        <v>56</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="B137" t="s">
+        <v>56</v>
+      </c>
+      <c r="C137" t="s">
         <v>96</v>
       </c>
-      <c r="D119" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120">
+      <c r="D137" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138">
         <v>970</v>
       </c>
-      <c r="B120" t="s">
-        <v>56</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="B138" t="s">
+        <v>56</v>
+      </c>
+      <c r="C138" t="s">
         <v>97</v>
       </c>
-      <c r="D120" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121">
+      <c r="D138" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139">
         <v>971</v>
       </c>
-      <c r="B121" t="s">
-        <v>56</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="B139" t="s">
+        <v>56</v>
+      </c>
+      <c r="C139" t="s">
         <v>99</v>
       </c>
-      <c r="D121" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122">
+      <c r="D139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140">
         <v>972</v>
       </c>
-      <c r="B122" t="s">
-        <v>56</v>
-      </c>
-      <c r="C122" t="s">
+      <c r="B140" t="s">
+        <v>56</v>
+      </c>
+      <c r="C140" t="s">
         <v>98</v>
       </c>
-      <c r="D122" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123">
+      <c r="D140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141">
         <v>973</v>
       </c>
-      <c r="B123" t="s">
-        <v>56</v>
-      </c>
-      <c r="C123" t="s">
+      <c r="B141" t="s">
+        <v>56</v>
+      </c>
+      <c r="C141" t="s">
         <v>100</v>
       </c>
-      <c r="D123" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124">
+      <c r="D141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142">
         <v>974</v>
       </c>
-      <c r="B124" t="s">
-        <v>56</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="B142" t="s">
+        <v>56</v>
+      </c>
+      <c r="C142" t="s">
         <v>101</v>
       </c>
-      <c r="D124" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125">
+      <c r="D142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143">
         <v>975</v>
       </c>
-      <c r="B125" t="s">
-        <v>56</v>
-      </c>
-      <c r="C125" t="s">
+      <c r="B143" t="s">
+        <v>56</v>
+      </c>
+      <c r="C143" t="s">
         <v>102</v>
       </c>
-      <c r="D125" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126">
+      <c r="D143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144">
         <v>976</v>
       </c>
-      <c r="B126" t="s">
-        <v>56</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B144" t="s">
+        <v>56</v>
+      </c>
+      <c r="C144" t="s">
         <v>103</v>
       </c>
-      <c r="D126" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127">
+      <c r="D144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145">
         <v>977</v>
       </c>
-      <c r="B127" t="s">
-        <v>56</v>
-      </c>
-      <c r="C127" t="s">
+      <c r="B145" t="s">
+        <v>56</v>
+      </c>
+      <c r="C145" t="s">
         <v>104</v>
       </c>
-      <c r="D127" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128">
+      <c r="D145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146">
         <v>978</v>
       </c>
-      <c r="B128" t="s">
-        <v>56</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="B146" t="s">
+        <v>56</v>
+      </c>
+      <c r="C146" t="s">
         <v>105</v>
       </c>
-      <c r="D128" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129">
+      <c r="D146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147">
         <v>979</v>
       </c>
-      <c r="B129" t="s">
-        <v>56</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="B147" t="s">
+        <v>56</v>
+      </c>
+      <c r="C147" t="s">
         <v>106</v>
       </c>
-      <c r="D129" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130">
+      <c r="D147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148">
         <v>980</v>
       </c>
-      <c r="B130" t="s">
-        <v>56</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="B148" t="s">
+        <v>56</v>
+      </c>
+      <c r="C148" t="s">
         <v>107</v>
       </c>
-      <c r="D130" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131">
+      <c r="D148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149">
         <v>981</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B149" t="s">
         <v>110</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C149" t="s">
         <v>109</v>
       </c>
-      <c r="D131" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132">
+      <c r="D149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150">
         <v>982</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B150" t="s">
         <v>110</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C150" t="s">
         <v>111</v>
       </c>
-      <c r="D132" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133">
+      <c r="D150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151">
         <v>983</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B151" t="s">
         <v>110</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C151" t="s">
         <v>112</v>
       </c>
-      <c r="D133" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134">
+      <c r="D151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152">
         <v>984</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B152" t="s">
         <v>110</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C152" t="s">
         <v>113</v>
       </c>
-      <c r="D134" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135">
+      <c r="D152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153">
         <v>985</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B153" t="s">
         <v>110</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C153" t="s">
         <v>114</v>
       </c>
-      <c r="D135" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136">
+      <c r="D153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154">
         <v>986</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B154" t="s">
         <v>110</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C154" t="s">
         <v>115</v>
       </c>
-      <c r="D136" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137">
+      <c r="D154" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155">
         <v>987</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B155" t="s">
         <v>110</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C155" t="s">
         <v>116</v>
       </c>
-      <c r="D137" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138">
+      <c r="D155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156">
         <v>988</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B156" t="s">
         <v>46</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C156" t="s">
         <v>117</v>
       </c>
-      <c r="D138" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139">
+      <c r="D156" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157">
         <v>989</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B157" t="s">
         <v>46</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C157" t="s">
         <v>118</v>
       </c>
-      <c r="D139" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140">
+      <c r="D157" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158">
         <v>990</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B158" t="s">
         <v>46</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C158" t="s">
         <v>119</v>
       </c>
-      <c r="D140" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141">
+      <c r="D158" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159">
         <v>991</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B159" t="s">
         <v>46</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C159" t="s">
         <v>120</v>
       </c>
-      <c r="D141" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142">
+      <c r="D159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160">
         <v>992</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B160" t="s">
         <v>46</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C160" t="s">
         <v>121</v>
       </c>
-      <c r="D142" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143">
+      <c r="D160" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161">
         <v>993</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B161" t="s">
         <v>122</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C161" t="s">
         <v>123</v>
       </c>
-      <c r="D143" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144">
+      <c r="D161" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162">
         <v>994</v>
       </c>
-      <c r="B144" t="s">
-        <v>56</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="B162" t="s">
+        <v>56</v>
+      </c>
+      <c r="C162" t="s">
         <v>124</v>
       </c>
-      <c r="D144" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145">
+      <c r="D162" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163">
         <v>995</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B163" t="s">
         <v>125</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C163" t="s">
         <v>126</v>
       </c>
-      <c r="D145" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146">
+      <c r="D163" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164">
         <v>996</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B164" t="s">
         <v>125</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C164" t="s">
         <v>127</v>
       </c>
-      <c r="D146" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147">
+      <c r="D164" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165">
         <v>997</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B165" t="s">
         <v>46</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C165" t="s">
         <v>128</v>
       </c>
-      <c r="D147" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148">
+      <c r="D165" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166">
         <v>998</v>
       </c>
-      <c r="B148" t="s">
-        <v>56</v>
-      </c>
-      <c r="C148" t="s">
+      <c r="B166" t="s">
+        <v>56</v>
+      </c>
+      <c r="C166" t="s">
         <v>129</v>
       </c>
-      <c r="D148" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149">
+      <c r="D166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167">
         <v>999</v>
       </c>
-      <c r="B149" t="s">
-        <v>56</v>
-      </c>
-      <c r="C149" t="s">
+      <c r="B167" t="s">
+        <v>56</v>
+      </c>
+      <c r="C167" t="s">
         <v>130</v>
       </c>
-      <c r="D149" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="D167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>53</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B168" t="s">
         <v>54</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C168" t="s">
         <v>55</v>
       </c>
-      <c r="D150" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>676</v>
-      </c>
-      <c r="B151" t="s">
-        <v>108</v>
-      </c>
-      <c r="C151" t="s">
-        <v>165</v>
-      </c>
-      <c r="D151" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>677</v>
-      </c>
-      <c r="B152" t="s">
-        <v>108</v>
-      </c>
-      <c r="C152" t="s">
-        <v>166</v>
-      </c>
-      <c r="D152" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>678</v>
-      </c>
-      <c r="B153" t="s">
-        <v>108</v>
-      </c>
-      <c r="C153" t="s">
-        <v>167</v>
-      </c>
-      <c r="D153" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>679</v>
-      </c>
-      <c r="B154" t="s">
-        <v>108</v>
-      </c>
-      <c r="C154" t="s">
-        <v>168</v>
-      </c>
-      <c r="D154" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>680</v>
-      </c>
-      <c r="B155" t="s">
-        <v>108</v>
-      </c>
-      <c r="C155" t="s">
-        <v>169</v>
-      </c>
-      <c r="D155" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <v>681</v>
-      </c>
-      <c r="B156" t="s">
-        <v>108</v>
-      </c>
-      <c r="C156" t="s">
-        <v>170</v>
-      </c>
-      <c r="D156" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <v>682</v>
-      </c>
-      <c r="B157" t="s">
-        <v>56</v>
-      </c>
-      <c r="C157" t="s">
-        <v>171</v>
-      </c>
-      <c r="D157" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <v>683</v>
-      </c>
-      <c r="B158" t="s">
-        <v>108</v>
-      </c>
-      <c r="C158" t="s">
-        <v>172</v>
-      </c>
-      <c r="D158" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <v>684</v>
-      </c>
-      <c r="B159" t="s">
-        <v>108</v>
-      </c>
-      <c r="C159" t="s">
-        <v>173</v>
-      </c>
-      <c r="D159" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>685</v>
-      </c>
-      <c r="B160" t="s">
-        <v>108</v>
-      </c>
-      <c r="C160" t="s">
-        <v>174</v>
-      </c>
-      <c r="D160" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>686</v>
-      </c>
-      <c r="B161" t="s">
-        <v>108</v>
-      </c>
-      <c r="C161" t="s">
-        <v>175</v>
-      </c>
-      <c r="D161" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>687</v>
-      </c>
-      <c r="B162" t="s">
-        <v>108</v>
-      </c>
-      <c r="C162" t="s">
-        <v>176</v>
-      </c>
-      <c r="D162" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163">
-        <v>688</v>
-      </c>
-      <c r="B163" t="s">
-        <v>108</v>
-      </c>
-      <c r="C163" t="s">
-        <v>177</v>
-      </c>
-      <c r="D163" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164">
-        <v>689</v>
-      </c>
-      <c r="B164" t="s">
-        <v>108</v>
-      </c>
-      <c r="C164" t="s">
-        <v>178</v>
-      </c>
-      <c r="D164" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>690</v>
-      </c>
-      <c r="B165" t="s">
-        <v>108</v>
-      </c>
-      <c r="C165" t="s">
-        <v>179</v>
-      </c>
-      <c r="D165" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>691</v>
-      </c>
-      <c r="B166" t="s">
-        <v>108</v>
-      </c>
-      <c r="C166" t="s">
-        <v>180</v>
-      </c>
-      <c r="D166" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167">
-        <v>692</v>
-      </c>
-      <c r="B167" t="s">
-        <v>56</v>
-      </c>
-      <c r="C167" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>693</v>
-      </c>
-      <c r="B168" t="s">
-        <v>56</v>
-      </c>
-      <c r="C168" t="s">
-        <v>182</v>
+      <c r="D168" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>626</v>
+      </c>
+      <c r="B169" t="s">
+        <v>110</v>
+      </c>
+      <c r="C169" t="s">
+        <v>183</v>
+      </c>
+      <c r="D169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>625</v>
+      </c>
+      <c r="B170" t="s">
+        <v>110</v>
+      </c>
+      <c r="C170" t="s">
+        <v>184</v>
+      </c>
+      <c r="D170" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>624</v>
+      </c>
+      <c r="B171" t="s">
+        <v>110</v>
+      </c>
+      <c r="C171" t="s">
+        <v>185</v>
+      </c>
+      <c r="D171" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2">
-    <sortState ref="A3:D150">
+    <sortState ref="A3:D168">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Force users to select a type of tree when creating a new tree.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="188">
   <si>
     <t>Number</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t>Currnetly Unadoptable  (Click to change)</t>
+  </si>
+  <si>
+    <t>Select a type of food</t>
+  </si>
+  <si>
+    <t>Please select a type of food.</t>
   </si>
 </sst>
 </file>
@@ -937,21 +943,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H171"/>
+  <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="C173" sqref="C173"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -961,7 +967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -978,7 +984,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -992,7 +998,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>90</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>91</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>92</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>93</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>100</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>101</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>200</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>201</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>202</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>203</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>204</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>205</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>206</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>300</v>
       </c>
@@ -1188,7 +1194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>301</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>302</v>
       </c>
@@ -1216,7 +1222,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>303</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>304</v>
       </c>
@@ -1244,7 +1250,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>305</v>
       </c>
@@ -1258,7 +1264,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>307</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>400</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>401</v>
       </c>
@@ -1300,7 +1306,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>402</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>403</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>404</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>405</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>406</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>407</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>408</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>409</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>410</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>411</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>412</v>
       </c>
@@ -1454,7 +1460,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>413</v>
       </c>
@@ -1468,7 +1474,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>414</v>
       </c>
@@ -1482,7 +1488,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>415</v>
       </c>
@@ -1496,7 +1502,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>416</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>417</v>
       </c>
@@ -1524,7 +1530,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>500</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>501</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>502</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>503</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>504</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>505</v>
       </c>
@@ -1608,7 +1614,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>601</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>602</v>
       </c>
@@ -1636,7 +1642,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>603</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>604</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>605</v>
       </c>
@@ -1678,7 +1684,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>606</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>607</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>608</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>609</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>610</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>611</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>612</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>613</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>627</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>628</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>629</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>630</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>631</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>632</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>633</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>634</v>
       </c>
@@ -1902,7 +1908,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>635</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>636</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>637</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>638</v>
       </c>
@@ -1958,7 +1964,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>639</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>640</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>641</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>662</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>663</v>
       </c>
@@ -2028,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>664</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>665</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>666</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>667</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>668</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>669</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>670</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>671</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>672</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>673</v>
       </c>
@@ -2168,7 +2174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>676</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>677</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>678</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>679</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>680</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>681</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>682</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>683</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>684</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>685</v>
       </c>
@@ -2308,7 +2314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>686</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>687</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>688</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>689</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>690</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>691</v>
       </c>
@@ -2392,7 +2398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>692</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>693</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>706</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>730</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>900</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>901</v>
       </c>
@@ -2470,7 +2476,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>902</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>903</v>
       </c>
@@ -2498,7 +2504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>904</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>905</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>906</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>929</v>
       </c>
@@ -2554,7 +2560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>930</v>
       </c>
@@ -2568,7 +2574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>931</v>
       </c>
@@ -2582,7 +2588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>932</v>
       </c>
@@ -2596,7 +2602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>933</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>934</v>
       </c>
@@ -2624,7 +2630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>935</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>936</v>
       </c>
@@ -2652,7 +2658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>937</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>938</v>
       </c>
@@ -2674,7 +2680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>939</v>
       </c>
@@ -2685,7 +2691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>940</v>
       </c>
@@ -2696,7 +2702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>941</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>960</v>
       </c>
@@ -2724,7 +2730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>961</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>962</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>963</v>
       </c>
@@ -2766,7 +2772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>964</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>965</v>
       </c>
@@ -2794,7 +2800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>966</v>
       </c>
@@ -2808,7 +2814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>967</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>968</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>969</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>970</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>971</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>972</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>973</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>974</v>
       </c>
@@ -2920,7 +2926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>975</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>976</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>977</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>978</v>
       </c>
@@ -2976,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>979</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>980</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>981</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>982</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>983</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>984</v>
       </c>
@@ -3060,7 +3066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>985</v>
       </c>
@@ -3074,7 +3080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>986</v>
       </c>
@@ -3088,7 +3094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>987</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>988</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>989</v>
       </c>
@@ -3130,7 +3136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>990</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>991</v>
       </c>
@@ -3158,7 +3164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>992</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>993</v>
       </c>
@@ -3186,7 +3192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>994</v>
       </c>
@@ -3200,7 +3206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>995</v>
       </c>
@@ -3214,7 +3220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>996</v>
       </c>
@@ -3228,7 +3234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>997</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>998</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>999</v>
       </c>
@@ -3270,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>53</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>626</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>625</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>624</v>
       </c>
@@ -3324,6 +3330,34 @@
       </c>
       <c r="D171" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>642</v>
+      </c>
+      <c r="B172" t="s">
+        <v>71</v>
+      </c>
+      <c r="C172" t="s">
+        <v>186</v>
+      </c>
+      <c r="D172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>643</v>
+      </c>
+      <c r="B173" t="s">
+        <v>71</v>
+      </c>
+      <c r="C173" t="s">
+        <v>187</v>
+      </c>
+      <c r="D173" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read image metadata to set the date of note/donate post automatically.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="190">
   <si>
     <t>Number</t>
   </si>
@@ -591,6 +591,12 @@
   </si>
   <si>
     <t>Please select a type of food.</t>
+  </si>
+  <si>
+    <t>Note/Donate</t>
+  </si>
+  <si>
+    <t>Date has been set</t>
   </si>
 </sst>
 </file>
@@ -943,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,13 +1804,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B61" t="s">
         <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
@@ -1812,13 +1818,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B62" t="s">
         <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="D62" t="s">
         <v>2</v>
@@ -1826,13 +1832,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B63" t="s">
         <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
@@ -1840,13 +1846,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B64" t="s">
         <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
@@ -1854,13 +1860,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B65" t="s">
         <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D65" t="s">
         <v>2</v>
@@ -1868,13 +1874,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B66" t="s">
         <v>110</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D66" t="s">
         <v>2</v>
@@ -1882,13 +1888,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D67" t="s">
         <v>2</v>
@@ -1896,41 +1902,41 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="D68" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C69" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B70" t="s">
         <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="D70" t="s">
         <v>2</v>
@@ -1938,13 +1944,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B71" t="s">
         <v>71</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D71" t="s">
         <v>62</v>
@@ -1952,13 +1958,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D72" t="s">
         <v>62</v>
@@ -1966,69 +1972,69 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="B73" t="s">
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D73" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B74" t="s">
         <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="D74" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B75" t="s">
         <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="D75" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>662</v>
+        <v>639</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>663</v>
+        <v>640</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D77" t="s">
         <v>2</v>
@@ -2036,69 +2042,69 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>664</v>
+        <v>641</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C78" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="D78" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>665</v>
+        <v>642</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C79" t="s">
-        <v>81</v>
+        <v>186</v>
       </c>
       <c r="D79" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>666</v>
+        <v>643</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="B81" t="s">
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="D81" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="B82" t="s">
         <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
         <v>2</v>
@@ -2106,41 +2112,41 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="B83" t="s">
         <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="B85" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>146</v>
+        <v>83</v>
       </c>
       <c r="D85" t="s">
         <v>2</v>
@@ -2148,27 +2154,27 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="B87" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C87" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D87" t="s">
         <v>2</v>
@@ -2176,13 +2182,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="B88" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C88" t="s">
-        <v>165</v>
+        <v>79</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
@@ -2190,13 +2196,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="C89" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D89" t="s">
         <v>2</v>
@@ -2204,13 +2210,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="C90" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
@@ -2218,13 +2224,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="C91" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
@@ -2232,13 +2238,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="C92" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D92" t="s">
         <v>2</v>
@@ -2246,13 +2252,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="B93" t="s">
         <v>108</v>
       </c>
       <c r="C93" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
@@ -2260,13 +2266,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="B94" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C94" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D94" t="s">
         <v>2</v>
@@ -2274,13 +2280,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="B95" t="s">
         <v>108</v>
       </c>
       <c r="C95" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D95" t="s">
         <v>2</v>
@@ -2288,13 +2294,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="B96" t="s">
         <v>108</v>
       </c>
       <c r="C96" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D96" t="s">
         <v>2</v>
@@ -2302,13 +2308,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="B97" t="s">
         <v>108</v>
       </c>
       <c r="C97" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D97" t="s">
         <v>2</v>
@@ -2316,13 +2322,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="B98" t="s">
         <v>108</v>
       </c>
       <c r="C98" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D98" t="s">
         <v>2</v>
@@ -2330,13 +2336,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="B99" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C99" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
@@ -2344,13 +2350,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="B100" t="s">
         <v>108</v>
       </c>
       <c r="C100" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D100" t="s">
         <v>2</v>
@@ -2358,13 +2364,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="B101" t="s">
         <v>108</v>
       </c>
       <c r="C101" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
@@ -2372,13 +2378,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="B102" t="s">
         <v>108</v>
       </c>
       <c r="C102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
@@ -2386,13 +2392,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="B103" t="s">
         <v>108</v>
       </c>
       <c r="C103" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
@@ -2400,35 +2406,41 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="B104" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C104" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="D104" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="B105" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C105" t="s">
-        <v>182</v>
+        <v>177</v>
+      </c>
+      <c r="D105" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>706</v>
+        <v>689</v>
       </c>
       <c r="B106" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -2436,13 +2448,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>730</v>
+        <v>690</v>
       </c>
       <c r="B107" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C107" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -2450,83 +2462,77 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>900</v>
+        <v>691</v>
       </c>
       <c r="B108" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="C108" t="s">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="D108" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>901</v>
+        <v>692</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C109" t="s">
-        <v>68</v>
-      </c>
-      <c r="D109" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>902</v>
+        <v>693</v>
       </c>
       <c r="B110" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>69</v>
-      </c>
-      <c r="D110" t="s">
-        <v>62</v>
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>903</v>
+        <v>706</v>
       </c>
       <c r="B111" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C111" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D111" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>904</v>
+        <v>730</v>
       </c>
       <c r="B112" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C112" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D112" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="B113" t="s">
         <v>45</v>
       </c>
       <c r="C113" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D113" t="s">
         <v>62</v>
@@ -2534,13 +2540,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="B114" t="s">
         <v>45</v>
       </c>
       <c r="C114" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D114" t="s">
         <v>62</v>
@@ -2548,83 +2554,83 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>929</v>
+        <v>902</v>
       </c>
       <c r="B115" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C115" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="D115" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>930</v>
+        <v>903</v>
       </c>
       <c r="B116" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C116" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="D116" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>931</v>
+        <v>904</v>
       </c>
       <c r="B117" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C117" t="s">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="D117" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>932</v>
+        <v>905</v>
       </c>
       <c r="B118" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C118" t="s">
-        <v>134</v>
+        <v>65</v>
       </c>
       <c r="D118" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>933</v>
+        <v>906</v>
       </c>
       <c r="B119" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C119" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="D119" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="B120" t="s">
         <v>56</v>
       </c>
       <c r="C120" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D120" t="s">
         <v>2</v>
@@ -2632,13 +2638,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="B121" t="s">
         <v>56</v>
       </c>
       <c r="C121" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D121" t="s">
         <v>2</v>
@@ -2646,13 +2652,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="B122" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="C122" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="D122" t="s">
         <v>2</v>
@@ -2660,10 +2666,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="B123" t="s">
-        <v>88</v>
+        <v>56</v>
+      </c>
+      <c r="C123" t="s">
+        <v>134</v>
       </c>
       <c r="D123" t="s">
         <v>2</v>
@@ -2671,10 +2680,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="B124" t="s">
-        <v>88</v>
+        <v>56</v>
+      </c>
+      <c r="C124" t="s">
+        <v>133</v>
       </c>
       <c r="D124" t="s">
         <v>2</v>
@@ -2682,10 +2694,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="B125" t="s">
-        <v>88</v>
+        <v>56</v>
+      </c>
+      <c r="C125" t="s">
+        <v>132</v>
       </c>
       <c r="D125" t="s">
         <v>2</v>
@@ -2693,10 +2708,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="B126" t="s">
-        <v>88</v>
+        <v>56</v>
+      </c>
+      <c r="C126" t="s">
+        <v>131</v>
       </c>
       <c r="D126" t="s">
         <v>2</v>
@@ -2704,13 +2722,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="B127" t="s">
         <v>88</v>
       </c>
       <c r="C127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D127" t="s">
         <v>2</v>
@@ -2718,13 +2736,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>960</v>
+        <v>937</v>
       </c>
       <c r="B128" t="s">
-        <v>56</v>
-      </c>
-      <c r="C128" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="D128" t="s">
         <v>2</v>
@@ -2732,13 +2747,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>961</v>
+        <v>938</v>
       </c>
       <c r="B129" t="s">
-        <v>56</v>
-      </c>
-      <c r="C129" t="s">
-        <v>156</v>
+        <v>88</v>
       </c>
       <c r="D129" t="s">
         <v>2</v>
@@ -2746,13 +2758,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>962</v>
+        <v>939</v>
       </c>
       <c r="B130" t="s">
-        <v>56</v>
-      </c>
-      <c r="C130" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D130" t="s">
         <v>2</v>
@@ -2760,13 +2769,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>963</v>
+        <v>940</v>
       </c>
       <c r="B131" t="s">
-        <v>56</v>
-      </c>
-      <c r="C131" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D131" t="s">
         <v>2</v>
@@ -2774,13 +2780,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>964</v>
+        <v>941</v>
       </c>
       <c r="B132" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C132" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D132" t="s">
         <v>2</v>
@@ -2788,13 +2794,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>965</v>
+        <v>960</v>
       </c>
       <c r="B133" t="s">
         <v>56</v>
       </c>
       <c r="C133" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="D133" t="s">
         <v>2</v>
@@ -2802,13 +2808,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="B134" t="s">
         <v>56</v>
       </c>
       <c r="C134" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D134" t="s">
         <v>2</v>
@@ -2816,13 +2822,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>967</v>
+        <v>962</v>
       </c>
       <c r="B135" t="s">
         <v>56</v>
       </c>
       <c r="C135" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D135" t="s">
         <v>2</v>
@@ -2830,13 +2836,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>968</v>
+        <v>963</v>
       </c>
       <c r="B136" t="s">
         <v>56</v>
       </c>
       <c r="C136" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D136" t="s">
         <v>2</v>
@@ -2844,13 +2850,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>969</v>
+        <v>964</v>
       </c>
       <c r="B137" t="s">
         <v>56</v>
       </c>
       <c r="C137" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D137" t="s">
         <v>2</v>
@@ -2858,13 +2864,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>970</v>
+        <v>965</v>
       </c>
       <c r="B138" t="s">
         <v>56</v>
       </c>
       <c r="C138" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
@@ -2872,13 +2878,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>971</v>
+        <v>966</v>
       </c>
       <c r="B139" t="s">
         <v>56</v>
       </c>
       <c r="C139" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="D139" t="s">
         <v>2</v>
@@ -2886,13 +2892,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>972</v>
+        <v>967</v>
       </c>
       <c r="B140" t="s">
         <v>56</v>
       </c>
       <c r="C140" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D140" t="s">
         <v>2</v>
@@ -2900,13 +2906,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>973</v>
+        <v>968</v>
       </c>
       <c r="B141" t="s">
         <v>56</v>
       </c>
       <c r="C141" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D141" t="s">
         <v>2</v>
@@ -2914,13 +2920,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>974</v>
+        <v>969</v>
       </c>
       <c r="B142" t="s">
         <v>56</v>
       </c>
       <c r="C142" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D142" t="s">
         <v>2</v>
@@ -2928,13 +2934,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>975</v>
+        <v>970</v>
       </c>
       <c r="B143" t="s">
         <v>56</v>
       </c>
       <c r="C143" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D143" t="s">
         <v>2</v>
@@ -2942,13 +2948,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>976</v>
+        <v>971</v>
       </c>
       <c r="B144" t="s">
         <v>56</v>
       </c>
       <c r="C144" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D144" t="s">
         <v>2</v>
@@ -2956,13 +2962,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>977</v>
+        <v>972</v>
       </c>
       <c r="B145" t="s">
         <v>56</v>
       </c>
       <c r="C145" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D145" t="s">
         <v>2</v>
@@ -2970,13 +2976,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>978</v>
+        <v>973</v>
       </c>
       <c r="B146" t="s">
         <v>56</v>
       </c>
       <c r="C146" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D146" t="s">
         <v>2</v>
@@ -2984,13 +2990,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>979</v>
+        <v>974</v>
       </c>
       <c r="B147" t="s">
         <v>56</v>
       </c>
       <c r="C147" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D147" t="s">
         <v>2</v>
@@ -2998,13 +3004,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>980</v>
+        <v>975</v>
       </c>
       <c r="B148" t="s">
         <v>56</v>
       </c>
       <c r="C148" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D148" t="s">
         <v>2</v>
@@ -3012,13 +3018,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>981</v>
+        <v>976</v>
       </c>
       <c r="B149" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C149" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D149" t="s">
         <v>2</v>
@@ -3026,13 +3032,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>982</v>
+        <v>977</v>
       </c>
       <c r="B150" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C150" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D150" t="s">
         <v>2</v>
@@ -3040,13 +3046,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="B151" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C151" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D151" t="s">
         <v>2</v>
@@ -3054,13 +3060,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>984</v>
+        <v>979</v>
       </c>
       <c r="B152" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C152" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D152" t="s">
         <v>2</v>
@@ -3068,13 +3074,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>985</v>
+        <v>980</v>
       </c>
       <c r="B153" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C153" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D153" t="s">
         <v>2</v>
@@ -3082,13 +3088,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>986</v>
+        <v>981</v>
       </c>
       <c r="B154" t="s">
         <v>110</v>
       </c>
       <c r="C154" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D154" t="s">
         <v>2</v>
@@ -3096,13 +3102,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>987</v>
+        <v>982</v>
       </c>
       <c r="B155" t="s">
         <v>110</v>
       </c>
       <c r="C155" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D155" t="s">
         <v>2</v>
@@ -3110,13 +3116,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>988</v>
+        <v>983</v>
       </c>
       <c r="B156" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C156" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D156" t="s">
         <v>2</v>
@@ -3124,13 +3130,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>989</v>
+        <v>984</v>
       </c>
       <c r="B157" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C157" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D157" t="s">
         <v>2</v>
@@ -3138,13 +3144,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>990</v>
+        <v>985</v>
       </c>
       <c r="B158" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C158" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D158" t="s">
         <v>2</v>
@@ -3152,13 +3158,13 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>991</v>
+        <v>986</v>
       </c>
       <c r="B159" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C159" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D159" t="s">
         <v>2</v>
@@ -3166,13 +3172,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>992</v>
+        <v>987</v>
       </c>
       <c r="B160" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C160" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D160" t="s">
         <v>2</v>
@@ -3180,13 +3186,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>993</v>
+        <v>988</v>
       </c>
       <c r="B161" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="C161" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D161" t="s">
         <v>2</v>
@@ -3194,13 +3200,13 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>994</v>
+        <v>989</v>
       </c>
       <c r="B162" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C162" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D162" t="s">
         <v>2</v>
@@ -3208,13 +3214,13 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>995</v>
+        <v>990</v>
       </c>
       <c r="B163" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="C163" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D163" t="s">
         <v>2</v>
@@ -3222,13 +3228,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>996</v>
+        <v>991</v>
       </c>
       <c r="B164" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="C164" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D164" t="s">
         <v>2</v>
@@ -3236,13 +3242,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>997</v>
+        <v>992</v>
       </c>
       <c r="B165" t="s">
         <v>46</v>
       </c>
       <c r="C165" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D165" t="s">
         <v>2</v>
@@ -3250,13 +3256,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>998</v>
+        <v>993</v>
       </c>
       <c r="B166" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="C166" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D166" t="s">
         <v>2</v>
@@ -3264,41 +3270,41 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>999</v>
+        <v>994</v>
       </c>
       <c r="B167" t="s">
         <v>56</v>
       </c>
       <c r="C167" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D167" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>53</v>
+      <c r="A168">
+        <v>995</v>
       </c>
       <c r="B168" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="C168" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="D168" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>626</v>
+        <v>996</v>
       </c>
       <c r="B169" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C169" t="s">
-        <v>183</v>
+        <v>127</v>
       </c>
       <c r="D169" t="s">
         <v>2</v>
@@ -3306,13 +3312,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>625</v>
+        <v>997</v>
       </c>
       <c r="B170" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C170" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="D170" t="s">
         <v>2</v>
@@ -3320,13 +3326,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>624</v>
+        <v>998</v>
       </c>
       <c r="B171" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C171" t="s">
-        <v>185</v>
+        <v>129</v>
       </c>
       <c r="D171" t="s">
         <v>2</v>
@@ -3334,35 +3340,49 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>642</v>
+        <v>999</v>
       </c>
       <c r="B172" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C172" t="s">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="D172" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>643</v>
+      <c r="A173" t="s">
+        <v>53</v>
       </c>
       <c r="B173" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C173" t="s">
-        <v>187</v>
+        <v>55</v>
       </c>
       <c r="D173" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>674</v>
+      </c>
+      <c r="B174" t="s">
+        <v>188</v>
+      </c>
+      <c r="C174" t="s">
+        <v>189</v>
+      </c>
+      <c r="D174" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2">
-    <sortState ref="A3:D168">
+    <sortState ref="A3:D173">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Add newly added tree id in the user's browser cookie so that user can edit or delete during 15 minutes.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="191">
   <si>
     <t>Number</t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>Date has been set</t>
+  </si>
+  <si>
+    <t>Temporarily allowed to edit this tree.</t>
   </si>
 </sst>
 </file>
@@ -949,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3378,6 +3381,20 @@
       </c>
       <c r="D174" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>675</v>
+      </c>
+      <c r="B175" t="s">
+        <v>71</v>
+      </c>
+      <c r="C175" t="s">
+        <v>190</v>
+      </c>
+      <c r="D175" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update compiled js file for /FoodParent2.0 url.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -605,7 +605,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -765,6 +765,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -800,6 +817,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -954,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on mail sending.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="194">
   <si>
     <t>Number</t>
   </si>
@@ -600,6 +600,15 @@
   </si>
   <si>
     <t>Temporarily allowed to edit this tree.</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>No valid recipient.</t>
+  </si>
+  <si>
+    <t>No matched tree.</t>
   </si>
 </sst>
 </file>
@@ -986,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3429,6 +3438,34 @@
       </c>
       <c r="D175" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>330</v>
+      </c>
+      <c r="B176" t="s">
+        <v>191</v>
+      </c>
+      <c r="C176" t="s">
+        <v>192</v>
+      </c>
+      <c r="D176" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>331</v>
+      </c>
+      <c r="B177" t="s">
+        <v>191</v>
+      </c>
+      <c r="C177" t="s">
+        <v>193</v>
+      </c>
+      <c r="D177" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add geolocation permission denied popup message.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FoodParent2.0\serverconfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\captainwhale52\OneDrive\Workspace\Web\FoodParent2.0\serverconfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="196">
   <si>
     <t>Number</t>
   </si>
@@ -609,6 +609,12 @@
   </si>
   <si>
     <t>No matched tree.</t>
+  </si>
+  <si>
+    <t>Geolocation</t>
+  </si>
+  <si>
+    <t>Geolocation permission is denied.</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H177"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,6 +3471,20 @@
         <v>193</v>
       </c>
       <c r="D177" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>332</v>
+      </c>
+      <c r="B178" t="s">
+        <v>194</v>
+      </c>
+      <c r="C178" t="s">
+        <v>195</v>
+      </c>
+      <c r="D178" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add phantomjs screenshot function.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on canvas markers.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add description & action buttons.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="209">
   <si>
     <t>Number</t>
   </si>
@@ -645,6 +645,15 @@
   </si>
   <si>
     <t>There are unsaved changes.</t>
+  </si>
+  <si>
+    <t>No description.</t>
+  </si>
+  <si>
+    <t>EDIT</t>
+  </si>
+  <si>
+    <t>* Danger Zone *</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H187"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3642,6 +3651,48 @@
       </c>
       <c r="D187" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>95</v>
+      </c>
+      <c r="B188" t="s">
+        <v>56</v>
+      </c>
+      <c r="C188" t="s">
+        <v>206</v>
+      </c>
+      <c r="D188" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>928</v>
+      </c>
+      <c r="B189" t="s">
+        <v>56</v>
+      </c>
+      <c r="C189" t="s">
+        <v>207</v>
+      </c>
+      <c r="D189" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>927</v>
+      </c>
+      <c r="B190" t="s">
+        <v>56</v>
+      </c>
+      <c r="C190" t="s">
+        <v>208</v>
+      </c>
+      <c r="D190" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on login form.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="212">
   <si>
     <t>Number</t>
   </si>
@@ -654,6 +654,15 @@
   </si>
   <si>
     <t>* Danger Zone *</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Contact (E-mail) cannot be modified.</t>
+  </si>
+  <si>
+    <t>Role can be only modified by manager.</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H190"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3692,6 +3701,48 @@
         <v>208</v>
       </c>
       <c r="D190" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>96</v>
+      </c>
+      <c r="B191" t="s">
+        <v>56</v>
+      </c>
+      <c r="C191" t="s">
+        <v>209</v>
+      </c>
+      <c r="D191" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>97</v>
+      </c>
+      <c r="B192" t="s">
+        <v>122</v>
+      </c>
+      <c r="C192" t="s">
+        <v>210</v>
+      </c>
+      <c r="D192" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>98</v>
+      </c>
+      <c r="B193" t="s">
+        <v>122</v>
+      </c>
+      <c r="C193" t="s">
+        <v>211</v>
+      </c>
+      <c r="D193" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on CRUD for Tree.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="215">
   <si>
     <t>Number</t>
   </si>
@@ -663,6 +663,15 @@
   </si>
   <si>
     <t>Role can be only modified by manager.</t>
+  </si>
+  <si>
+    <t>Cancel adding a new tree.</t>
+  </si>
+  <si>
+    <t>See parent info.</t>
+  </si>
+  <si>
+    <t>* You are allowed to edit information of the tree for 15 minutes.</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:H196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="B193" sqref="B193"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3743,6 +3752,48 @@
         <v>211</v>
       </c>
       <c r="D193" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>79</v>
+      </c>
+      <c r="B194" t="s">
+        <v>197</v>
+      </c>
+      <c r="C194" t="s">
+        <v>212</v>
+      </c>
+      <c r="D194" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>78</v>
+      </c>
+      <c r="B195" t="s">
+        <v>197</v>
+      </c>
+      <c r="C195" t="s">
+        <v>213</v>
+      </c>
+      <c r="D195" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>77</v>
+      </c>
+      <c r="B196" t="s">
+        <v>71</v>
+      </c>
+      <c r="C196" t="s">
+        <v>214</v>
+      </c>
+      <c r="D196" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on the note detail.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="218">
   <si>
     <t>Number</t>
   </si>
@@ -675,6 +675,12 @@
   </si>
   <si>
     <t>No flag.</t>
+  </si>
+  <si>
+    <t>PICK UP</t>
+  </si>
+  <si>
+    <t>Note Type</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H197"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3811,6 +3817,48 @@
         <v>215</v>
       </c>
       <c r="D197" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>75</v>
+      </c>
+      <c r="B198" t="s">
+        <v>46</v>
+      </c>
+      <c r="C198" t="s">
+        <v>216</v>
+      </c>
+      <c r="D198" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>74</v>
+      </c>
+      <c r="B199" t="s">
+        <v>46</v>
+      </c>
+      <c r="C199" t="s">
+        <v>132</v>
+      </c>
+      <c r="D199" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>73</v>
+      </c>
+      <c r="B200" t="s">
+        <v>46</v>
+      </c>
+      <c r="C200" t="s">
+        <v>217</v>
+      </c>
+      <c r="D200" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change info panel menu style.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="225">
   <si>
     <t>Number</t>
   </si>
@@ -699,6 +699,9 @@
   </si>
   <si>
     <t>No photos.</t>
+  </si>
+  <si>
+    <t>Double click for full screen mode.</t>
   </si>
 </sst>
 </file>
@@ -1085,9 +1088,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H205"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
       <selection activeCell="C205" sqref="C205"/>
     </sheetView>
   </sheetViews>
@@ -3945,6 +3948,23 @@
       </c>
       <c r="C205" t="s">
         <v>223</v>
+      </c>
+      <c r="D205" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>68</v>
+      </c>
+      <c r="B206" t="s">
+        <v>125</v>
+      </c>
+      <c r="C206" t="s">
+        <v>224</v>
+      </c>
+      <c r="D206" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add image delete button.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="226">
   <si>
     <t>Number</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>Double click for full screen mode.</t>
+  </si>
+  <si>
+    <t>DELETE SELECTED PHOTO</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H206"/>
+  <dimension ref="A1:H207"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="C205" sqref="C205"/>
+      <selection activeCell="B207" sqref="B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3965,6 +3968,17 @@
       </c>
       <c r="D206" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>67</v>
+      </c>
+      <c r="B207" t="s">
+        <v>125</v>
+      </c>
+      <c r="C207" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add dead field in tree table, and connect to add tree, filter.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="229">
   <si>
     <t>Number</t>
   </si>
@@ -705,6 +705,15 @@
   </si>
   <si>
     <t>DELETE SELECTED PHOTO</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>*Unkown</t>
+  </si>
+  <si>
+    <t>Tree doesn't exist or access is restricted.</t>
   </si>
 </sst>
 </file>
@@ -1091,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H207"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="B207" sqref="B207"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="C208" sqref="C208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3979,6 +3988,37 @@
       </c>
       <c r="C207" t="s">
         <v>225</v>
+      </c>
+      <c r="D207" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>66</v>
+      </c>
+      <c r="B208" t="s">
+        <v>226</v>
+      </c>
+      <c r="C208" t="s">
+        <v>227</v>
+      </c>
+      <c r="D208" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>65</v>
+      </c>
+      <c r="B209" t="s">
+        <v>71</v>
+      </c>
+      <c r="C209" t="s">
+        <v>228</v>
+      </c>
+      <c r="D209" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add note author field.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="231">
   <si>
     <t>Number</t>
   </si>
@@ -714,6 +714,12 @@
   </si>
   <si>
     <t>Tree doesn't exist or access is restricted.</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Anonymous</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H209"/>
+  <dimension ref="A1:H211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="C214" sqref="C214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4018,6 +4024,34 @@
         <v>228</v>
       </c>
       <c r="D209" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>64</v>
+      </c>
+      <c r="B210" t="s">
+        <v>46</v>
+      </c>
+      <c r="C210" t="s">
+        <v>229</v>
+      </c>
+      <c r="D210" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>63</v>
+      </c>
+      <c r="B211" t="s">
+        <v>46</v>
+      </c>
+      <c r="C211" t="s">
+        <v>230</v>
+      </c>
+      <c r="D211" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on the recent post.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="234">
   <si>
     <t>Number</t>
   </si>
@@ -720,6 +720,15 @@
   </si>
   <si>
     <t>Anonymous</t>
+  </si>
+  <si>
+    <t>Recent Post</t>
+  </si>
+  <si>
+    <t>Recent Pickup</t>
+  </si>
+  <si>
+    <t>Recent Donation</t>
   </si>
 </sst>
 </file>
@@ -1106,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="C214" sqref="C214"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4052,6 +4061,48 @@
         <v>230</v>
       </c>
       <c r="D211" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>62</v>
+      </c>
+      <c r="B212" t="s">
+        <v>46</v>
+      </c>
+      <c r="C212" t="s">
+        <v>231</v>
+      </c>
+      <c r="D212" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>61</v>
+      </c>
+      <c r="B213" t="s">
+        <v>46</v>
+      </c>
+      <c r="C213" t="s">
+        <v>232</v>
+      </c>
+      <c r="D213" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>60</v>
+      </c>
+      <c r="B214" t="s">
+        <v>84</v>
+      </c>
+      <c r="C214" t="s">
+        <v>233</v>
+      </c>
+      <c r="D214" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tree adopt / un-adopt function.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="239">
   <si>
     <t>Number</t>
   </si>
@@ -738,6 +738,12 @@
   </si>
   <si>
     <t>No recent donate.</t>
+  </si>
+  <si>
+    <t>You have adopted this tree.</t>
+  </si>
+  <si>
+    <t>You and</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H217"/>
+  <dimension ref="A1:H219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="E217" sqref="E217"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="C217" sqref="C217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,6 +4160,34 @@
         <v>236</v>
       </c>
       <c r="D217" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>56</v>
+      </c>
+      <c r="B218" t="s">
+        <v>110</v>
+      </c>
+      <c r="C218" t="s">
+        <v>237</v>
+      </c>
+      <c r="D218" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>55</v>
+      </c>
+      <c r="B219" t="s">
+        <v>110</v>
+      </c>
+      <c r="C219" t="s">
+        <v>238</v>
+      </c>
+      <c r="D219" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on donation note.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="245">
   <si>
     <t>Number</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>No name.</t>
+  </si>
+  <si>
+    <t>from</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H224"/>
+  <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="C223" sqref="C223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4273,6 +4276,20 @@
         <v>243</v>
       </c>
       <c r="D224" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>49</v>
+      </c>
+      <c r="B225" t="s">
+        <v>84</v>
+      </c>
+      <c r="C225" t="s">
+        <v>244</v>
+      </c>
+      <c r="D225" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add filter reset buton.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="252">
   <si>
     <t>Number</t>
   </si>
@@ -780,6 +780,9 @@
   </si>
   <si>
     <t>New Tree Info</t>
+  </si>
+  <si>
+    <t>In-Season/Upcoming Foods</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H231"/>
+  <dimension ref="A1:H232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C231" sqref="C231"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,6 +4396,17 @@
       </c>
       <c r="D231" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>42</v>
+      </c>
+      <c r="B232" t="s">
+        <v>225</v>
+      </c>
+      <c r="C232" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a recent donation section to the tree info panel.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="253">
   <si>
     <t>Number</t>
   </si>
@@ -783,6 +783,9 @@
   </si>
   <si>
     <t>In-Season/Upcoming Foods</t>
+  </si>
+  <si>
+    <t>to</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H232"/>
+  <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="C234" sqref="C234"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="C233" sqref="C233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4407,6 +4410,23 @@
       </c>
       <c r="C232" t="s">
         <v>251</v>
+      </c>
+      <c r="D232" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>41</v>
+      </c>
+      <c r="B233" t="s">
+        <v>84</v>
+      </c>
+      <c r="C233" t="s">
+        <v>252</v>
+      </c>
+      <c r="D233" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove typescript files & show both note and donate data on tree history panel.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="255">
   <si>
     <t>Number</t>
   </si>
@@ -170,12 +170,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Not a number value.</t>
-  </si>
-  <si>
-    <t>Negative number value.</t>
-  </si>
-  <si>
     <t>Account is already exist.</t>
   </si>
   <si>
@@ -786,6 +780,18 @@
   </si>
   <si>
     <t>to</t>
+  </si>
+  <si>
+    <t>Unknown Recipient</t>
+  </si>
+  <si>
+    <t>Please choose at least one tree source.</t>
+  </si>
+  <si>
+    <t>Please use a positive number.</t>
+  </si>
+  <si>
+    <t>Please use a number value.</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H233"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="C233" sqref="C233"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,12 +1194,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,10 +1227,10 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1232,13 +1238,13 @@
         <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1246,13 +1252,13 @@
         <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1260,13 +1266,13 @@
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1274,13 +1280,13 @@
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1294,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1308,7 +1314,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1322,7 +1328,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1336,7 +1342,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1350,7 +1356,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1364,7 +1370,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1378,7 +1384,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1392,7 +1398,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1406,7 +1412,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1440,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,7 +1454,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,7 +1468,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,7 +1482,7 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,7 +1496,7 @@
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1510,7 @@
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,7 +1524,7 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,7 +1538,7 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,7 +1552,7 @@
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,7 +1580,7 @@
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,7 +1594,7 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,7 +1608,7 @@
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,7 +1622,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,7 +1636,7 @@
         <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,7 +1650,7 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,7 +1664,7 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,7 +1678,7 @@
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,7 +1692,7 @@
         <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1700,7 +1706,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1714,7 +1720,7 @@
         <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1728,7 +1734,7 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1742,7 +1748,7 @@
         <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,7 +1762,7 @@
         <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1770,7 +1776,7 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +1790,7 @@
         <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,7 +1804,7 @@
         <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,7 +1818,7 @@
         <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,7 +1832,7 @@
         <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,7 +1846,7 @@
         <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1848,10 +1854,10 @@
         <v>601</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -1862,13 +1868,13 @@
         <v>602</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>253</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,13 +1882,13 @@
         <v>603</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>254</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,10 +1899,10 @@
         <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,10 +1913,10 @@
         <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1921,7 +1927,7 @@
         <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>2</v>
@@ -1935,10 +1941,10 @@
         <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,10 +1952,10 @@
         <v>608</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -1960,10 +1966,10 @@
         <v>609</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D56" t="s">
         <v>2</v>
@@ -1974,10 +1980,10 @@
         <v>610</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D57" t="s">
         <v>2</v>
@@ -1988,10 +1994,10 @@
         <v>611</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
@@ -2002,10 +2008,10 @@
         <v>612</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
@@ -2016,10 +2022,10 @@
         <v>613</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
@@ -2030,10 +2036,10 @@
         <v>624</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
@@ -2044,10 +2050,10 @@
         <v>625</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C62" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D62" t="s">
         <v>2</v>
@@ -2058,10 +2064,10 @@
         <v>626</v>
       </c>
       <c r="B63" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
@@ -2072,10 +2078,10 @@
         <v>627</v>
       </c>
       <c r="B64" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
@@ -2086,10 +2092,10 @@
         <v>628</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D65" t="s">
         <v>2</v>
@@ -2100,10 +2106,10 @@
         <v>629</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C66" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D66" t="s">
         <v>2</v>
@@ -2114,10 +2120,10 @@
         <v>630</v>
       </c>
       <c r="B67" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D67" t="s">
         <v>2</v>
@@ -2128,10 +2134,10 @@
         <v>631</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D68" t="s">
         <v>2</v>
@@ -2142,10 +2148,10 @@
         <v>632</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D69" t="s">
         <v>2</v>
@@ -2156,10 +2162,10 @@
         <v>633</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D70" t="s">
         <v>2</v>
@@ -2170,13 +2176,13 @@
         <v>634</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,13 +2190,13 @@
         <v>635</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D72" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,10 +2204,10 @@
         <v>636</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D73" t="s">
         <v>2</v>
@@ -2212,13 +2218,13 @@
         <v>637</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,13 +2232,13 @@
         <v>638</v>
       </c>
       <c r="B75" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" t="s">
         <v>71</v>
       </c>
-      <c r="C75" t="s">
-        <v>73</v>
-      </c>
       <c r="D75" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,13 +2246,13 @@
         <v>639</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D76" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,10 +2260,10 @@
         <v>640</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D77" t="s">
         <v>2</v>
@@ -2268,10 +2274,10 @@
         <v>641</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D78" t="s">
         <v>2</v>
@@ -2282,10 +2288,10 @@
         <v>642</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C79" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D79" t="s">
         <v>2</v>
@@ -2296,13 +2302,13 @@
         <v>643</v>
       </c>
       <c r="B80" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D80" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,10 +2316,10 @@
         <v>663</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D81" t="s">
         <v>2</v>
@@ -2324,10 +2330,10 @@
         <v>662</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D82" t="s">
         <v>2</v>
@@ -2338,13 +2344,13 @@
         <v>664</v>
       </c>
       <c r="B83" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C83" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D83" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,13 +2358,13 @@
         <v>665</v>
       </c>
       <c r="B84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
         <v>79</v>
       </c>
-      <c r="C84" t="s">
-        <v>81</v>
-      </c>
       <c r="D84" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,10 +2372,10 @@
         <v>666</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C85" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D85" t="s">
         <v>2</v>
@@ -2380,13 +2386,13 @@
         <v>667</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C86" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D86" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,10 +2400,10 @@
         <v>668</v>
       </c>
       <c r="B87" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C87" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D87" t="s">
         <v>2</v>
@@ -2408,10 +2414,10 @@
         <v>669</v>
       </c>
       <c r="B88" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C88" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
@@ -2425,7 +2431,7 @@
         <v>46</v>
       </c>
       <c r="C89" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D89" t="s">
         <v>2</v>
@@ -2439,7 +2445,7 @@
         <v>46</v>
       </c>
       <c r="C90" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
@@ -2453,7 +2459,7 @@
         <v>46</v>
       </c>
       <c r="C91" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
@@ -2467,7 +2473,7 @@
         <v>46</v>
       </c>
       <c r="C92" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D92" t="s">
         <v>2</v>
@@ -2478,10 +2484,10 @@
         <v>676</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
@@ -2492,10 +2498,10 @@
         <v>677</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C94" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D94" t="s">
         <v>2</v>
@@ -2506,10 +2512,10 @@
         <v>678</v>
       </c>
       <c r="B95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C95" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D95" t="s">
         <v>2</v>
@@ -2520,10 +2526,10 @@
         <v>679</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C96" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D96" t="s">
         <v>2</v>
@@ -2534,10 +2540,10 @@
         <v>680</v>
       </c>
       <c r="B97" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C97" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D97" t="s">
         <v>2</v>
@@ -2548,10 +2554,10 @@
         <v>681</v>
       </c>
       <c r="B98" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C98" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D98" t="s">
         <v>2</v>
@@ -2562,10 +2568,10 @@
         <v>682</v>
       </c>
       <c r="B99" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C99" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
@@ -2576,10 +2582,10 @@
         <v>683</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C100" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D100" t="s">
         <v>2</v>
@@ -2590,10 +2596,10 @@
         <v>684</v>
       </c>
       <c r="B101" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C101" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
@@ -2604,10 +2610,10 @@
         <v>685</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
@@ -2618,10 +2624,10 @@
         <v>686</v>
       </c>
       <c r="B103" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
@@ -2632,10 +2638,10 @@
         <v>687</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
@@ -2646,10 +2652,10 @@
         <v>688</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -2660,10 +2666,10 @@
         <v>689</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C106" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -2674,10 +2680,10 @@
         <v>690</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -2688,10 +2694,10 @@
         <v>691</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D108" t="s">
         <v>2</v>
@@ -2702,10 +2708,10 @@
         <v>692</v>
       </c>
       <c r="B109" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C109" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,10 +2719,10 @@
         <v>693</v>
       </c>
       <c r="B110" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C110" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2724,10 +2730,10 @@
         <v>706</v>
       </c>
       <c r="B111" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C111" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D111" t="s">
         <v>2</v>
@@ -2738,10 +2744,10 @@
         <v>730</v>
       </c>
       <c r="B112" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C112" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D112" t="s">
         <v>2</v>
@@ -2758,7 +2764,7 @@
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2769,10 +2775,10 @@
         <v>45</v>
       </c>
       <c r="C114" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D114" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2783,10 +2789,10 @@
         <v>45</v>
       </c>
       <c r="C115" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D115" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2797,10 +2803,10 @@
         <v>45</v>
       </c>
       <c r="C116" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D116" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2811,10 +2817,10 @@
         <v>45</v>
       </c>
       <c r="C117" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D117" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2825,10 +2831,10 @@
         <v>45</v>
       </c>
       <c r="C118" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D118" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,10 +2845,10 @@
         <v>45</v>
       </c>
       <c r="C119" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D119" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2850,10 +2856,10 @@
         <v>929</v>
       </c>
       <c r="B120" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C120" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D120" t="s">
         <v>2</v>
@@ -2864,10 +2870,10 @@
         <v>930</v>
       </c>
       <c r="B121" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C121" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D121" t="s">
         <v>2</v>
@@ -2878,10 +2884,10 @@
         <v>931</v>
       </c>
       <c r="B122" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C122" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D122" t="s">
         <v>2</v>
@@ -2892,10 +2898,10 @@
         <v>932</v>
       </c>
       <c r="B123" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C123" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D123" t="s">
         <v>2</v>
@@ -2906,10 +2912,10 @@
         <v>933</v>
       </c>
       <c r="B124" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C124" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D124" t="s">
         <v>2</v>
@@ -2920,10 +2926,10 @@
         <v>934</v>
       </c>
       <c r="B125" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C125" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D125" t="s">
         <v>2</v>
@@ -2934,10 +2940,10 @@
         <v>935</v>
       </c>
       <c r="B126" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C126" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D126" t="s">
         <v>2</v>
@@ -2948,10 +2954,10 @@
         <v>936</v>
       </c>
       <c r="B127" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C127" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D127" t="s">
         <v>2</v>
@@ -2962,7 +2968,7 @@
         <v>937</v>
       </c>
       <c r="B128" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D128" t="s">
         <v>2</v>
@@ -2973,7 +2979,7 @@
         <v>938</v>
       </c>
       <c r="B129" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D129" t="s">
         <v>2</v>
@@ -2984,7 +2990,7 @@
         <v>939</v>
       </c>
       <c r="B130" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D130" t="s">
         <v>2</v>
@@ -2995,7 +3001,7 @@
         <v>940</v>
       </c>
       <c r="B131" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D131" t="s">
         <v>2</v>
@@ -3006,10 +3012,10 @@
         <v>941</v>
       </c>
       <c r="B132" t="s">
+        <v>86</v>
+      </c>
+      <c r="C132" t="s">
         <v>88</v>
-      </c>
-      <c r="C132" t="s">
-        <v>90</v>
       </c>
       <c r="D132" t="s">
         <v>2</v>
@@ -3020,10 +3026,10 @@
         <v>960</v>
       </c>
       <c r="B133" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C133" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D133" t="s">
         <v>2</v>
@@ -3034,10 +3040,10 @@
         <v>961</v>
       </c>
       <c r="B134" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C134" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D134" t="s">
         <v>2</v>
@@ -3048,10 +3054,10 @@
         <v>962</v>
       </c>
       <c r="B135" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C135" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D135" t="s">
         <v>2</v>
@@ -3062,10 +3068,10 @@
         <v>963</v>
       </c>
       <c r="B136" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C136" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D136" t="s">
         <v>2</v>
@@ -3076,10 +3082,10 @@
         <v>964</v>
       </c>
       <c r="B137" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C137" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D137" t="s">
         <v>2</v>
@@ -3090,10 +3096,10 @@
         <v>965</v>
       </c>
       <c r="B138" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C138" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
@@ -3104,10 +3110,10 @@
         <v>966</v>
       </c>
       <c r="B139" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C139" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D139" t="s">
         <v>2</v>
@@ -3118,10 +3124,10 @@
         <v>967</v>
       </c>
       <c r="B140" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C140" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D140" t="s">
         <v>2</v>
@@ -3132,10 +3138,10 @@
         <v>968</v>
       </c>
       <c r="B141" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C141" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D141" t="s">
         <v>2</v>
@@ -3146,10 +3152,10 @@
         <v>969</v>
       </c>
       <c r="B142" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C142" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D142" t="s">
         <v>2</v>
@@ -3160,10 +3166,10 @@
         <v>970</v>
       </c>
       <c r="B143" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C143" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D143" t="s">
         <v>2</v>
@@ -3174,10 +3180,10 @@
         <v>971</v>
       </c>
       <c r="B144" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C144" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D144" t="s">
         <v>2</v>
@@ -3188,10 +3194,10 @@
         <v>972</v>
       </c>
       <c r="B145" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C145" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D145" t="s">
         <v>2</v>
@@ -3202,10 +3208,10 @@
         <v>973</v>
       </c>
       <c r="B146" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C146" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D146" t="s">
         <v>2</v>
@@ -3216,10 +3222,10 @@
         <v>974</v>
       </c>
       <c r="B147" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C147" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D147" t="s">
         <v>2</v>
@@ -3230,10 +3236,10 @@
         <v>975</v>
       </c>
       <c r="B148" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C148" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D148" t="s">
         <v>2</v>
@@ -3244,10 +3250,10 @@
         <v>976</v>
       </c>
       <c r="B149" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C149" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D149" t="s">
         <v>2</v>
@@ -3258,10 +3264,10 @@
         <v>977</v>
       </c>
       <c r="B150" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C150" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D150" t="s">
         <v>2</v>
@@ -3272,10 +3278,10 @@
         <v>978</v>
       </c>
       <c r="B151" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C151" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D151" t="s">
         <v>2</v>
@@ -3286,10 +3292,10 @@
         <v>979</v>
       </c>
       <c r="B152" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C152" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D152" t="s">
         <v>2</v>
@@ -3300,10 +3306,10 @@
         <v>980</v>
       </c>
       <c r="B153" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C153" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D153" t="s">
         <v>2</v>
@@ -3314,10 +3320,10 @@
         <v>981</v>
       </c>
       <c r="B154" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C154" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D154" t="s">
         <v>2</v>
@@ -3328,10 +3334,10 @@
         <v>982</v>
       </c>
       <c r="B155" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C155" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D155" t="s">
         <v>2</v>
@@ -3342,10 +3348,10 @@
         <v>983</v>
       </c>
       <c r="B156" t="s">
+        <v>108</v>
+      </c>
+      <c r="C156" t="s">
         <v>110</v>
-      </c>
-      <c r="C156" t="s">
-        <v>112</v>
       </c>
       <c r="D156" t="s">
         <v>2</v>
@@ -3356,10 +3362,10 @@
         <v>984</v>
       </c>
       <c r="B157" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C157" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D157" t="s">
         <v>2</v>
@@ -3370,10 +3376,10 @@
         <v>985</v>
       </c>
       <c r="B158" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C158" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D158" t="s">
         <v>2</v>
@@ -3384,10 +3390,10 @@
         <v>986</v>
       </c>
       <c r="B159" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C159" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D159" t="s">
         <v>2</v>
@@ -3398,10 +3404,10 @@
         <v>987</v>
       </c>
       <c r="B160" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D160" t="s">
         <v>2</v>
@@ -3415,7 +3421,7 @@
         <v>46</v>
       </c>
       <c r="C161" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D161" t="s">
         <v>2</v>
@@ -3429,7 +3435,7 @@
         <v>46</v>
       </c>
       <c r="C162" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D162" t="s">
         <v>2</v>
@@ -3443,7 +3449,7 @@
         <v>46</v>
       </c>
       <c r="C163" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D163" t="s">
         <v>2</v>
@@ -3457,7 +3463,7 @@
         <v>46</v>
       </c>
       <c r="C164" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D164" t="s">
         <v>2</v>
@@ -3471,7 +3477,7 @@
         <v>46</v>
       </c>
       <c r="C165" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D165" t="s">
         <v>2</v>
@@ -3482,10 +3488,10 @@
         <v>993</v>
       </c>
       <c r="B166" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C166" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D166" t="s">
         <v>2</v>
@@ -3496,10 +3502,10 @@
         <v>994</v>
       </c>
       <c r="B167" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C167" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D167" t="s">
         <v>2</v>
@@ -3510,10 +3516,10 @@
         <v>995</v>
       </c>
       <c r="B168" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C168" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D168" t="s">
         <v>2</v>
@@ -3524,10 +3530,10 @@
         <v>996</v>
       </c>
       <c r="B169" t="s">
+        <v>123</v>
+      </c>
+      <c r="C169" t="s">
         <v>125</v>
-      </c>
-      <c r="C169" t="s">
-        <v>127</v>
       </c>
       <c r="D169" t="s">
         <v>2</v>
@@ -3541,7 +3547,7 @@
         <v>46</v>
       </c>
       <c r="C170" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D170" t="s">
         <v>2</v>
@@ -3552,10 +3558,10 @@
         <v>998</v>
       </c>
       <c r="B171" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C171" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D171" t="s">
         <v>2</v>
@@ -3566,10 +3572,10 @@
         <v>999</v>
       </c>
       <c r="B172" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C172" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D172" t="s">
         <v>2</v>
@@ -3577,16 +3583,16 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>51</v>
+      </c>
+      <c r="B173" t="s">
+        <v>52</v>
+      </c>
+      <c r="C173" t="s">
         <v>53</v>
       </c>
-      <c r="B173" t="s">
-        <v>54</v>
-      </c>
-      <c r="C173" t="s">
-        <v>55</v>
-      </c>
       <c r="D173" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -3594,13 +3600,13 @@
         <v>674</v>
       </c>
       <c r="B174" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C174" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D174" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -3608,10 +3614,10 @@
         <v>675</v>
       </c>
       <c r="B175" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C175" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D175" t="s">
         <v>2</v>
@@ -3622,13 +3628,13 @@
         <v>330</v>
       </c>
       <c r="B176" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C176" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D176" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -3636,13 +3642,13 @@
         <v>331</v>
       </c>
       <c r="B177" t="s">
+        <v>188</v>
+      </c>
+      <c r="C177" t="s">
         <v>190</v>
       </c>
-      <c r="C177" t="s">
-        <v>192</v>
-      </c>
       <c r="D177" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -3650,13 +3656,13 @@
         <v>332</v>
       </c>
       <c r="B178" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C178" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D178" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -3664,13 +3670,13 @@
         <v>80</v>
       </c>
       <c r="B179" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C179" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D179" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -3678,13 +3684,13 @@
         <v>81</v>
       </c>
       <c r="B180" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C180" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D180" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3692,13 +3698,13 @@
         <v>82</v>
       </c>
       <c r="B181" t="s">
+        <v>194</v>
+      </c>
+      <c r="C181" t="s">
         <v>196</v>
       </c>
-      <c r="C181" t="s">
-        <v>198</v>
-      </c>
       <c r="D181" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3706,13 +3712,13 @@
         <v>83</v>
       </c>
       <c r="B182" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C182" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D182" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3720,13 +3726,13 @@
         <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C183" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D183" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -3734,13 +3740,13 @@
         <v>85</v>
       </c>
       <c r="B184" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C184" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D184" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3748,13 +3754,13 @@
         <v>86</v>
       </c>
       <c r="B185" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C185" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D185" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3762,13 +3768,13 @@
         <v>87</v>
       </c>
       <c r="B186" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C186" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D186" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,13 +3782,13 @@
         <v>94</v>
       </c>
       <c r="B187" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C187" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D187" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -3790,10 +3796,10 @@
         <v>95</v>
       </c>
       <c r="B188" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C188" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D188" t="s">
         <v>2</v>
@@ -3804,10 +3810,10 @@
         <v>928</v>
       </c>
       <c r="B189" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C189" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D189" t="s">
         <v>2</v>
@@ -3818,10 +3824,10 @@
         <v>927</v>
       </c>
       <c r="B190" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C190" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D190" t="s">
         <v>2</v>
@@ -3832,10 +3838,10 @@
         <v>96</v>
       </c>
       <c r="B191" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C191" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D191" t="s">
         <v>2</v>
@@ -3846,10 +3852,10 @@
         <v>97</v>
       </c>
       <c r="B192" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C192" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D192" t="s">
         <v>2</v>
@@ -3860,10 +3866,10 @@
         <v>98</v>
       </c>
       <c r="B193" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C193" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D193" t="s">
         <v>2</v>
@@ -3874,13 +3880,13 @@
         <v>79</v>
       </c>
       <c r="B194" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C194" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D194" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -3888,13 +3894,13 @@
         <v>78</v>
       </c>
       <c r="B195" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C195" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D195" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,10 +3908,10 @@
         <v>77</v>
       </c>
       <c r="B196" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C196" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D196" t="s">
         <v>2</v>
@@ -3916,10 +3922,10 @@
         <v>76</v>
       </c>
       <c r="B197" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C197" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D197" t="s">
         <v>2</v>
@@ -3933,7 +3939,7 @@
         <v>46</v>
       </c>
       <c r="C198" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D198" t="s">
         <v>2</v>
@@ -3947,7 +3953,7 @@
         <v>46</v>
       </c>
       <c r="C199" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D199" t="s">
         <v>2</v>
@@ -3961,7 +3967,7 @@
         <v>46</v>
       </c>
       <c r="C200" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D200" t="s">
         <v>2</v>
@@ -3972,10 +3978,10 @@
         <v>72</v>
       </c>
       <c r="B201" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C201" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D201" t="s">
         <v>2</v>
@@ -3989,7 +3995,7 @@
         <v>46</v>
       </c>
       <c r="C202" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D202" t="s">
         <v>2</v>
@@ -4000,10 +4006,10 @@
         <v>70</v>
       </c>
       <c r="B203" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C203" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D203" t="s">
         <v>2</v>
@@ -4014,10 +4020,10 @@
         <v>506</v>
       </c>
       <c r="B204" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C204" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D204" t="s">
         <v>2</v>
@@ -4028,10 +4034,10 @@
         <v>69</v>
       </c>
       <c r="B205" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C205" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D205" t="s">
         <v>2</v>
@@ -4042,10 +4048,10 @@
         <v>68</v>
       </c>
       <c r="B206" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C206" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D206" t="s">
         <v>2</v>
@@ -4056,10 +4062,10 @@
         <v>67</v>
       </c>
       <c r="B207" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C207" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D207" t="s">
         <v>2</v>
@@ -4070,10 +4076,10 @@
         <v>66</v>
       </c>
       <c r="B208" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C208" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D208" t="s">
         <v>2</v>
@@ -4084,10 +4090,10 @@
         <v>65</v>
       </c>
       <c r="B209" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C209" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D209" t="s">
         <v>2</v>
@@ -4101,7 +4107,7 @@
         <v>46</v>
       </c>
       <c r="C210" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D210" t="s">
         <v>2</v>
@@ -4115,7 +4121,7 @@
         <v>46</v>
       </c>
       <c r="C211" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D211" t="s">
         <v>2</v>
@@ -4129,7 +4135,7 @@
         <v>46</v>
       </c>
       <c r="C212" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D212" t="s">
         <v>2</v>
@@ -4143,7 +4149,7 @@
         <v>46</v>
       </c>
       <c r="C213" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D213" t="s">
         <v>2</v>
@@ -4154,10 +4160,10 @@
         <v>60</v>
       </c>
       <c r="B214" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C214" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D214" t="s">
         <v>2</v>
@@ -4171,7 +4177,7 @@
         <v>46</v>
       </c>
       <c r="C215" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D215" t="s">
         <v>2</v>
@@ -4185,7 +4191,7 @@
         <v>46</v>
       </c>
       <c r="C216" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D216" t="s">
         <v>2</v>
@@ -4196,10 +4202,10 @@
         <v>57</v>
       </c>
       <c r="B217" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C217" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D217" t="s">
         <v>2</v>
@@ -4210,10 +4216,10 @@
         <v>56</v>
       </c>
       <c r="B218" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C218" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D218" t="s">
         <v>2</v>
@@ -4224,10 +4230,10 @@
         <v>55</v>
       </c>
       <c r="B219" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C219" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D219" t="s">
         <v>2</v>
@@ -4238,13 +4244,13 @@
         <v>54</v>
       </c>
       <c r="B220" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C220" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D220" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -4252,13 +4258,13 @@
         <v>53</v>
       </c>
       <c r="B221" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C221" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D221" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,13 +4272,13 @@
         <v>52</v>
       </c>
       <c r="B222" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C222" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D222" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -4280,13 +4286,13 @@
         <v>51</v>
       </c>
       <c r="B223" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C223" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D223" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -4294,10 +4300,10 @@
         <v>50</v>
       </c>
       <c r="B224" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C224" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D224" t="s">
         <v>2</v>
@@ -4308,10 +4314,10 @@
         <v>49</v>
       </c>
       <c r="B225" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C225" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D225" t="s">
         <v>2</v>
@@ -4322,10 +4328,10 @@
         <v>48</v>
       </c>
       <c r="B226" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C226" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D226" t="s">
         <v>2</v>
@@ -4336,10 +4342,10 @@
         <v>47</v>
       </c>
       <c r="B227" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C227" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D227" t="s">
         <v>2</v>
@@ -4350,10 +4356,10 @@
         <v>46</v>
       </c>
       <c r="B228" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C228" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D228" t="s">
         <v>2</v>
@@ -4364,10 +4370,10 @@
         <v>45</v>
       </c>
       <c r="B229" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C229" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D229" t="s">
         <v>2</v>
@@ -4378,10 +4384,10 @@
         <v>44</v>
       </c>
       <c r="B230" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C230" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D230" t="s">
         <v>2</v>
@@ -4392,10 +4398,10 @@
         <v>43</v>
       </c>
       <c r="B231" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C231" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D231" t="s">
         <v>2</v>
@@ -4406,10 +4412,10 @@
         <v>42</v>
       </c>
       <c r="B232" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C232" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D232" t="s">
         <v>2</v>
@@ -4420,12 +4426,40 @@
         <v>41</v>
       </c>
       <c r="B233" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C233" t="s">
+        <v>250</v>
+      </c>
+      <c r="D233" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>40</v>
+      </c>
+      <c r="B234" t="s">
+        <v>82</v>
+      </c>
+      <c r="C234" t="s">
+        <v>251</v>
+      </c>
+      <c r="D234" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>39</v>
+      </c>
+      <c r="B235" t="s">
+        <v>82</v>
+      </c>
+      <c r="C235" t="s">
         <v>252</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D235" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add pickup & donate graph.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="259">
   <si>
     <t>Number</t>
   </si>
@@ -792,6 +792,18 @@
   </si>
   <si>
     <t>Please use a number value.</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Rating Update Graph</t>
+  </si>
+  <si>
+    <t>Pickup Amount Graph (accum. / year)</t>
+  </si>
+  <si>
+    <t>Donation Amount Graph (accum. / year)</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H235"/>
+  <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4460,6 +4472,48 @@
         <v>252</v>
       </c>
       <c r="D235" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>38</v>
+      </c>
+      <c r="B236" t="s">
+        <v>255</v>
+      </c>
+      <c r="C236" t="s">
+        <v>256</v>
+      </c>
+      <c r="D236" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>37</v>
+      </c>
+      <c r="B237" t="s">
+        <v>255</v>
+      </c>
+      <c r="C237" t="s">
+        <v>257</v>
+      </c>
+      <c r="D237" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>36</v>
+      </c>
+      <c r="B238" t="s">
+        <v>255</v>
+      </c>
+      <c r="C238" t="s">
+        <v>258</v>
+      </c>
+      <c r="D238" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add notification mailing system.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="269">
   <si>
     <t>Number</t>
   </si>
@@ -804,6 +804,36 @@
   </si>
   <si>
     <t>Donation Amount Graph (accum. / year)</t>
+  </si>
+  <si>
+    <t>Notify</t>
+  </si>
+  <si>
+    <t>NOTIFICATION</t>
+  </si>
+  <si>
+    <t>Past Pick-ups</t>
+  </si>
+  <si>
+    <t>Upcoming Trees</t>
+  </si>
+  <si>
+    <t>Notify Checked Trees to Managers</t>
+  </si>
+  <si>
+    <t>Notify Checked Trees to Parents</t>
+  </si>
+  <si>
+    <t>Failed to send a notification to parents.</t>
+  </si>
+  <si>
+    <t>Failed to send a notification to managers.</t>
+  </si>
+  <si>
+    <t>Server internal error. Please try again.</t>
+  </si>
+  <si>
+    <t>Notification has sent successfully.</t>
   </si>
 </sst>
 </file>
@@ -1190,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H238"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="C234" sqref="C234"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="C244" sqref="C244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4514,6 +4544,132 @@
         <v>258</v>
       </c>
       <c r="D238" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>35</v>
+      </c>
+      <c r="B239" t="s">
+        <v>259</v>
+      </c>
+      <c r="C239" t="s">
+        <v>260</v>
+      </c>
+      <c r="D239" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>34</v>
+      </c>
+      <c r="B240" t="s">
+        <v>259</v>
+      </c>
+      <c r="C240" t="s">
+        <v>261</v>
+      </c>
+      <c r="D240" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>33</v>
+      </c>
+      <c r="B241" t="s">
+        <v>259</v>
+      </c>
+      <c r="C241" t="s">
+        <v>262</v>
+      </c>
+      <c r="D241" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>32</v>
+      </c>
+      <c r="B242" t="s">
+        <v>259</v>
+      </c>
+      <c r="C242" t="s">
+        <v>263</v>
+      </c>
+      <c r="D242" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>31</v>
+      </c>
+      <c r="B243" t="s">
+        <v>259</v>
+      </c>
+      <c r="C243" t="s">
+        <v>264</v>
+      </c>
+      <c r="D243" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>30</v>
+      </c>
+      <c r="B244" t="s">
+        <v>259</v>
+      </c>
+      <c r="C244" t="s">
+        <v>268</v>
+      </c>
+      <c r="D244" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>29</v>
+      </c>
+      <c r="B245" t="s">
+        <v>259</v>
+      </c>
+      <c r="C245" t="s">
+        <v>265</v>
+      </c>
+      <c r="D245" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>28</v>
+      </c>
+      <c r="B246" t="s">
+        <v>259</v>
+      </c>
+      <c r="C246" t="s">
+        <v>266</v>
+      </c>
+      <c r="D246" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>27</v>
+      </c>
+      <c r="B247" t="s">
+        <v>259</v>
+      </c>
+      <c r="C247" t="s">
+        <v>267</v>
+      </c>
+      <c r="D247" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplify marker system & Fix media query for the info panel.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="C244" sqref="C244"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="C242" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change flag into dead / alive.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="270">
   <si>
     <t>Number</t>
   </si>
@@ -834,6 +834,9 @@
   </si>
   <si>
     <t>Notification has sent successfully.</t>
+  </si>
+  <si>
+    <t>No source tree.</t>
   </si>
 </sst>
 </file>
@@ -1220,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H247"/>
+  <dimension ref="A1:H248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="C242" sqref="C242"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4670,6 +4673,20 @@
         <v>267</v>
       </c>
       <c r="D247" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>26</v>
+      </c>
+      <c r="B248" t="s">
+        <v>82</v>
+      </c>
+      <c r="C248" t="s">
+        <v>269</v>
+      </c>
+      <c r="D248" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add image exif restorer (not fully functional).
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="273">
   <si>
     <t>Number</t>
   </si>
@@ -837,6 +837,15 @@
   </si>
   <si>
     <t>No source tree.</t>
+  </si>
+  <si>
+    <t>dead</t>
+  </si>
+  <si>
+    <t>alive</t>
+  </si>
+  <si>
+    <t>Uploading…</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H248"/>
+  <dimension ref="A1:H251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="C246" sqref="C246"/>
+    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="C251" sqref="C251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4687,6 +4696,48 @@
         <v>269</v>
       </c>
       <c r="D248" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>25</v>
+      </c>
+      <c r="B249" t="s">
+        <v>69</v>
+      </c>
+      <c r="C249" t="s">
+        <v>270</v>
+      </c>
+      <c r="D249" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>24</v>
+      </c>
+      <c r="B250" t="s">
+        <v>69</v>
+      </c>
+      <c r="C250" t="s">
+        <v>271</v>
+      </c>
+      <c r="D250" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>23</v>
+      </c>
+      <c r="B251" t="s">
+        <v>123</v>
+      </c>
+      <c r="C251" t="s">
+        <v>272</v>
+      </c>
+      <c r="D251" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix donation line location css word-break issue.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="275">
   <si>
     <t>Number</t>
   </si>
@@ -846,6 +846,12 @@
   </si>
   <si>
     <t>Uploading…</t>
+  </si>
+  <si>
+    <t>Food adoption status has been updated.</t>
+  </si>
+  <si>
+    <t>person have adopted this tree.</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H251"/>
+  <dimension ref="A1:H253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4738,6 +4744,34 @@
         <v>272</v>
       </c>
       <c r="D251" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>22</v>
+      </c>
+      <c r="B252" t="s">
+        <v>108</v>
+      </c>
+      <c r="C252" t="s">
+        <v>273</v>
+      </c>
+      <c r="D252" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>21</v>
+      </c>
+      <c r="B253" t="s">
+        <v>108</v>
+      </c>
+      <c r="C253" t="s">
+        <v>274</v>
+      </c>
+      <c r="D253" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change flex margin auto to specific number (IE fix).
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="276">
   <si>
     <t>Number</t>
   </si>
@@ -852,6 +852,9 @@
   </si>
   <si>
     <t>person have adopted this tree.</t>
+  </si>
+  <si>
+    <t>Not a valid image format.</t>
   </si>
 </sst>
 </file>
@@ -1238,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H253"/>
+  <dimension ref="A1:H254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="C253" sqref="C253"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,629 +1298,629 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>274</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>273</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>272</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>271</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>100</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>270</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>269</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>200</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
+      <c r="A10">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" t="s">
+        <v>267</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>201</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>202</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>203</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>268</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>204</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>264</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>205</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>263</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>206</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>262</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>300</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>261</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>301</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>260</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>302</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>258</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>303</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>304</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>256</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>305</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>252</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>400</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>20</v>
+      <c r="A24">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>250</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>401</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>223</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>249</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>402</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>403</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>247</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>404</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>246</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>405</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>245</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>406</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>244</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>407</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>243</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>408</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>242</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>409</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>241</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>410</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>411</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>237</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>412</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
+        <v>236</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>413</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>238</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>414</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>235</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>415</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>416</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>233</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>417</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>232</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>500</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>231</v>
       </c>
       <c r="D42" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>501</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>502</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>229</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>503</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>504</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>227</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>505</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>226</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>601</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -1925,69 +1928,69 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>602</v>
+        <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>223</v>
       </c>
       <c r="C49" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="D49" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>603</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>604</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>221</v>
       </c>
       <c r="D51" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>605</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>606</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>217</v>
       </c>
       <c r="D53" t="s">
         <v>2</v>
@@ -1995,27 +1998,27 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>607</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
         <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>216</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>608</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2023,13 +2026,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>609</v>
+        <v>73</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="D56" t="s">
         <v>2</v>
@@ -2037,13 +2040,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>610</v>
+        <v>74</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="D57" t="s">
         <v>2</v>
@@ -2051,13 +2054,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>611</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
@@ -2065,13 +2068,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>612</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>212</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
@@ -2079,13 +2082,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>613</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>211</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
@@ -2093,153 +2096,153 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>624</v>
+        <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="D61" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>625</v>
+        <v>79</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C62" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="D62" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>626</v>
+        <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C63" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D63" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>627</v>
+        <v>81</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>628</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C65" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>629</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>630</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C67" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>631</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C68" t="s">
-        <v>148</v>
+        <v>199</v>
       </c>
       <c r="D68" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>632</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="D69" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>633</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>194</v>
       </c>
       <c r="C70" t="s">
-        <v>147</v>
+        <v>201</v>
       </c>
       <c r="D70" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>634</v>
+        <v>90</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D71" t="s">
         <v>60</v>
@@ -2247,13 +2250,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>635</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D72" t="s">
         <v>60</v>
@@ -2261,27 +2264,27 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>636</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D73" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>637</v>
+        <v>93</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C74" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D74" t="s">
         <v>60</v>
@@ -2289,13 +2292,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>638</v>
+        <v>94</v>
       </c>
       <c r="B75" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>71</v>
+        <v>202</v>
       </c>
       <c r="D75" t="s">
         <v>60</v>
@@ -2303,27 +2306,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>639</v>
+        <v>95</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C76" t="s">
-        <v>72</v>
+        <v>203</v>
       </c>
       <c r="D76" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>640</v>
+        <v>96</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="D77" t="s">
         <v>2</v>
@@ -2331,13 +2334,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>641</v>
+        <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>135</v>
+        <v>207</v>
       </c>
       <c r="D78" t="s">
         <v>2</v>
@@ -2345,27 +2348,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>642</v>
+        <v>98</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="C79" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="D79" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>643</v>
-      </c>
-      <c r="B80" t="s">
-        <v>69</v>
-      </c>
-      <c r="C80" t="s">
-        <v>184</v>
+      <c r="A80" s="4">
+        <v>100</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D80" t="s">
         <v>60</v>
@@ -2373,41 +2376,41 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>663</v>
+        <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C81" t="s">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>662</v>
-      </c>
-      <c r="B82" t="s">
-        <v>77</v>
-      </c>
-      <c r="C82" t="s">
-        <v>139</v>
+      <c r="A82" s="1">
+        <v>200</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>664</v>
+        <v>201</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C83" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="D83" t="s">
         <v>60</v>
@@ -2415,13 +2418,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>665</v>
+        <v>202</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C84" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="D84" t="s">
         <v>60</v>
@@ -2429,27 +2432,27 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>666</v>
+        <v>203</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C85" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>667</v>
+        <v>204</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C86" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="D86" t="s">
         <v>60</v>
@@ -2457,371 +2460,377 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>668</v>
+        <v>205</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C87" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>669</v>
+        <v>206</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C88" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="D88" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>670</v>
+        <v>300</v>
       </c>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C89" t="s">
-        <v>143</v>
+        <v>13</v>
       </c>
       <c r="D89" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>671</v>
+        <v>301</v>
       </c>
       <c r="B90" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C90" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>672</v>
+        <v>302</v>
       </c>
       <c r="B91" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C91" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="D91" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>673</v>
+        <v>303</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C92" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>676</v>
+        <v>304</v>
       </c>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C93" t="s">
-        <v>163</v>
+        <v>17</v>
       </c>
       <c r="D93" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>677</v>
+        <v>305</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C94" t="s">
-        <v>164</v>
+        <v>18</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>678</v>
+        <v>307</v>
       </c>
       <c r="B95" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C95" t="s">
-        <v>165</v>
+        <v>19</v>
       </c>
       <c r="D95" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>679</v>
+        <v>330</v>
       </c>
       <c r="B96" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="C96" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="D96" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>680</v>
+        <v>331</v>
       </c>
       <c r="B97" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="C97" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="D97" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>681</v>
+        <v>332</v>
       </c>
       <c r="B98" t="s">
-        <v>106</v>
+        <v>191</v>
       </c>
       <c r="C98" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="D98" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>682</v>
-      </c>
-      <c r="B99" t="s">
-        <v>54</v>
-      </c>
-      <c r="C99" t="s">
-        <v>169</v>
+      <c r="A99" s="2">
+        <v>400</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D99" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>683</v>
+        <v>401</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>170</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>684</v>
+        <v>402</v>
       </c>
       <c r="B101" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C101" t="s">
-        <v>171</v>
+        <v>22</v>
       </c>
       <c r="D101" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>685</v>
+        <v>403</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C102" t="s">
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="D102" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>686</v>
+        <v>404</v>
       </c>
       <c r="B103" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C103" t="s">
-        <v>173</v>
+        <v>24</v>
       </c>
       <c r="D103" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>687</v>
+        <v>405</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C104" t="s">
-        <v>174</v>
+        <v>25</v>
       </c>
       <c r="D104" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>688</v>
+        <v>406</v>
       </c>
       <c r="B105" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C105" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="D105" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>689</v>
+        <v>407</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C106" t="s">
-        <v>176</v>
+        <v>27</v>
       </c>
       <c r="D106" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>690</v>
+        <v>408</v>
       </c>
       <c r="B107" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C107" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="D107" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>691</v>
+        <v>409</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C108" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="D108" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>692</v>
+        <v>410</v>
       </c>
       <c r="B109" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C109" t="s">
-        <v>179</v>
+        <v>30</v>
+      </c>
+      <c r="D109" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>693</v>
+        <v>411</v>
       </c>
       <c r="B110" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C110" t="s">
-        <v>239</v>
+        <v>31</v>
+      </c>
+      <c r="D110" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>706</v>
+        <v>412</v>
       </c>
       <c r="B111" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="C111" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="D111" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>730</v>
+        <v>413</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="C112" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>900</v>
+        <v>414</v>
       </c>
       <c r="B113" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C113" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D113" t="s">
         <v>60</v>
@@ -2829,13 +2838,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>901</v>
+        <v>415</v>
       </c>
       <c r="B114" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C114" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="D114" t="s">
         <v>60</v>
@@ -2843,13 +2852,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>902</v>
+        <v>416</v>
       </c>
       <c r="B115" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C115" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D115" t="s">
         <v>60</v>
@@ -2857,13 +2866,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>903</v>
+        <v>417</v>
       </c>
       <c r="B116" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C116" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D116" t="s">
         <v>60</v>
@@ -2871,13 +2880,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>904</v>
+        <v>500</v>
       </c>
       <c r="B117" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C117" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D117" t="s">
         <v>60</v>
@@ -2885,13 +2894,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>905</v>
+        <v>501</v>
       </c>
       <c r="B118" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C118" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D118" t="s">
         <v>60</v>
@@ -2899,13 +2908,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>906</v>
+        <v>502</v>
       </c>
       <c r="B119" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C119" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D119" t="s">
         <v>60</v>
@@ -2913,55 +2922,55 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>929</v>
+        <v>503</v>
       </c>
       <c r="B120" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C120" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="D120" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>930</v>
+        <v>504</v>
       </c>
       <c r="B121" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C121" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="D121" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>931</v>
+        <v>505</v>
       </c>
       <c r="B122" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C122" t="s">
-        <v>133</v>
+        <v>43</v>
       </c>
       <c r="D122" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>932</v>
+        <v>506</v>
       </c>
       <c r="B123" t="s">
-        <v>54</v>
+        <v>218</v>
       </c>
       <c r="C123" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="D123" t="s">
         <v>2</v>
@@ -2969,13 +2978,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>933</v>
+        <v>601</v>
       </c>
       <c r="B124" t="s">
         <v>54</v>
       </c>
       <c r="C124" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="D124" t="s">
         <v>2</v>
@@ -2983,63 +2992,69 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>934</v>
+        <v>602</v>
       </c>
       <c r="B125" t="s">
         <v>54</v>
       </c>
       <c r="C125" t="s">
-        <v>130</v>
+        <v>253</v>
       </c>
       <c r="D125" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>935</v>
+        <v>603</v>
       </c>
       <c r="B126" t="s">
         <v>54</v>
       </c>
       <c r="C126" t="s">
-        <v>129</v>
+        <v>254</v>
       </c>
       <c r="D126" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>936</v>
+        <v>604</v>
       </c>
       <c r="B127" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C127" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D127" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>937</v>
+        <v>605</v>
       </c>
       <c r="B128" t="s">
-        <v>86</v>
+        <v>46</v>
+      </c>
+      <c r="C128" t="s">
+        <v>74</v>
       </c>
       <c r="D128" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>938</v>
+        <v>606</v>
       </c>
       <c r="B129" t="s">
-        <v>86</v>
+        <v>46</v>
+      </c>
+      <c r="C129" t="s">
+        <v>61</v>
       </c>
       <c r="D129" t="s">
         <v>2</v>
@@ -3047,21 +3062,27 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>939</v>
+        <v>607</v>
       </c>
       <c r="B130" t="s">
-        <v>86</v>
+        <v>46</v>
+      </c>
+      <c r="C130" t="s">
+        <v>65</v>
       </c>
       <c r="D130" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>940</v>
+        <v>608</v>
       </c>
       <c r="B131" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="C131" t="s">
+        <v>162</v>
       </c>
       <c r="D131" t="s">
         <v>2</v>
@@ -3069,13 +3090,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>941</v>
+        <v>609</v>
       </c>
       <c r="B132" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C132" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="D132" t="s">
         <v>2</v>
@@ -3083,13 +3104,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>960</v>
+        <v>610</v>
       </c>
       <c r="B133" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C133" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D133" t="s">
         <v>2</v>
@@ -3097,13 +3118,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>961</v>
+        <v>611</v>
       </c>
       <c r="B134" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C134" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D134" t="s">
         <v>2</v>
@@ -3111,13 +3132,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>962</v>
+        <v>612</v>
       </c>
       <c r="B135" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C135" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="D135" t="s">
         <v>2</v>
@@ -3125,13 +3146,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>963</v>
+        <v>613</v>
       </c>
       <c r="B136" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C136" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="D136" t="s">
         <v>2</v>
@@ -3139,13 +3160,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>964</v>
+        <v>624</v>
       </c>
       <c r="B137" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C137" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="D137" t="s">
         <v>2</v>
@@ -3153,13 +3174,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>965</v>
+        <v>625</v>
       </c>
       <c r="B138" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C138" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
@@ -3167,13 +3188,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>966</v>
+        <v>626</v>
       </c>
       <c r="B139" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C139" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="D139" t="s">
         <v>2</v>
@@ -3181,13 +3202,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>967</v>
+        <v>627</v>
       </c>
       <c r="B140" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C140" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="D140" t="s">
         <v>2</v>
@@ -3195,13 +3216,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>968</v>
+        <v>628</v>
       </c>
       <c r="B141" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C141" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="D141" t="s">
         <v>2</v>
@@ -3209,13 +3230,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>969</v>
+        <v>629</v>
       </c>
       <c r="B142" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C142" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="D142" t="s">
         <v>2</v>
@@ -3223,13 +3244,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>970</v>
+        <v>630</v>
       </c>
       <c r="B143" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C143" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="D143" t="s">
         <v>2</v>
@@ -3237,13 +3258,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>971</v>
+        <v>631</v>
       </c>
       <c r="B144" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C144" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D144" t="s">
         <v>2</v>
@@ -3251,13 +3272,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>972</v>
+        <v>632</v>
       </c>
       <c r="B145" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C145" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="D145" t="s">
         <v>2</v>
@@ -3265,13 +3286,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>973</v>
+        <v>633</v>
       </c>
       <c r="B146" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C146" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="D146" t="s">
         <v>2</v>
@@ -3279,41 +3300,41 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>974</v>
+        <v>634</v>
       </c>
       <c r="B147" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C147" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D147" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>975</v>
+        <v>635</v>
       </c>
       <c r="B148" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C148" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="D148" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>976</v>
+        <v>636</v>
       </c>
       <c r="B149" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C149" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D149" t="s">
         <v>2</v>
@@ -3321,55 +3342,55 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>977</v>
+        <v>637</v>
       </c>
       <c r="B150" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C150" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="D150" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>978</v>
+        <v>638</v>
       </c>
       <c r="B151" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C151" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D151" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>979</v>
+        <v>639</v>
       </c>
       <c r="B152" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C152" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="D152" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>980</v>
+        <v>640</v>
       </c>
       <c r="B153" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C153" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="D153" t="s">
         <v>2</v>
@@ -3377,13 +3398,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>981</v>
+        <v>641</v>
       </c>
       <c r="B154" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="C154" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="D154" t="s">
         <v>2</v>
@@ -3391,13 +3412,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>982</v>
+        <v>642</v>
       </c>
       <c r="B155" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="C155" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="D155" t="s">
         <v>2</v>
@@ -3405,27 +3426,27 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>983</v>
+        <v>643</v>
       </c>
       <c r="B156" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="C156" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="D156" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>984</v>
+        <v>662</v>
       </c>
       <c r="B157" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C157" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="D157" t="s">
         <v>2</v>
@@ -3433,13 +3454,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>985</v>
+        <v>663</v>
       </c>
       <c r="B158" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C158" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D158" t="s">
         <v>2</v>
@@ -3447,41 +3468,41 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>986</v>
+        <v>664</v>
       </c>
       <c r="B159" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C159" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="D159" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>987</v>
+        <v>665</v>
       </c>
       <c r="B160" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C160" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="D160" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>988</v>
+        <v>666</v>
       </c>
       <c r="B161" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C161" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="D161" t="s">
         <v>2</v>
@@ -3489,27 +3510,27 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>989</v>
+        <v>667</v>
       </c>
       <c r="B162" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C162" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="D162" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>990</v>
+        <v>668</v>
       </c>
       <c r="B163" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C163" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="D163" t="s">
         <v>2</v>
@@ -3517,13 +3538,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>991</v>
+        <v>669</v>
       </c>
       <c r="B164" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C164" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="D164" t="s">
         <v>2</v>
@@ -3531,13 +3552,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>992</v>
+        <v>670</v>
       </c>
       <c r="B165" t="s">
         <v>46</v>
       </c>
       <c r="C165" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="D165" t="s">
         <v>2</v>
@@ -3545,13 +3566,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>993</v>
+        <v>671</v>
       </c>
       <c r="B166" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="C166" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="D166" t="s">
         <v>2</v>
@@ -3559,13 +3580,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>994</v>
+        <v>672</v>
       </c>
       <c r="B167" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C167" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="D167" t="s">
         <v>2</v>
@@ -3573,13 +3594,13 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>995</v>
+        <v>673</v>
       </c>
       <c r="B168" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="C168" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D168" t="s">
         <v>2</v>
@@ -3587,27 +3608,27 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>996</v>
+        <v>674</v>
       </c>
       <c r="B169" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="C169" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="D169" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>997</v>
+        <v>675</v>
       </c>
       <c r="B170" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C170" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="D170" t="s">
         <v>2</v>
@@ -3615,13 +3636,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>998</v>
+        <v>676</v>
       </c>
       <c r="B171" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C171" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="D171" t="s">
         <v>2</v>
@@ -3629,55 +3650,55 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>999</v>
+        <v>677</v>
       </c>
       <c r="B172" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C172" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="D172" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>51</v>
+      <c r="A173">
+        <v>678</v>
       </c>
       <c r="B173" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="C173" t="s">
-        <v>53</v>
+        <v>165</v>
       </c>
       <c r="D173" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="B174" t="s">
-        <v>185</v>
+        <v>106</v>
       </c>
       <c r="C174" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D174" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="B175" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="C175" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="D175" t="s">
         <v>2</v>
@@ -3685,195 +3706,189 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>330</v>
+        <v>681</v>
       </c>
       <c r="B176" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="C176" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="D176" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>331</v>
+        <v>682</v>
       </c>
       <c r="B177" t="s">
-        <v>188</v>
+        <v>54</v>
       </c>
       <c r="C177" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D177" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>332</v>
+        <v>683</v>
       </c>
       <c r="B178" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="C178" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="D178" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>80</v>
+        <v>684</v>
       </c>
       <c r="B179" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C179" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="D179" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>81</v>
+        <v>685</v>
       </c>
       <c r="B180" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C180" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="D180" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>82</v>
+        <v>686</v>
       </c>
       <c r="B181" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C181" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="D181" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>83</v>
+        <v>687</v>
       </c>
       <c r="B182" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C182" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="D182" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>84</v>
+        <v>688</v>
       </c>
       <c r="B183" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C183" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="D183" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>85</v>
+        <v>689</v>
       </c>
       <c r="B184" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C184" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="D184" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>86</v>
+        <v>690</v>
       </c>
       <c r="B185" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C185" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="D185" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>87</v>
+        <v>691</v>
       </c>
       <c r="B186" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="C186" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="D186" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>94</v>
+        <v>692</v>
       </c>
       <c r="B187" t="s">
         <v>54</v>
       </c>
       <c r="C187" t="s">
-        <v>202</v>
-      </c>
-      <c r="D187" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>95</v>
+        <v>693</v>
       </c>
       <c r="B188" t="s">
         <v>54</v>
       </c>
       <c r="C188" t="s">
-        <v>203</v>
-      </c>
-      <c r="D188" t="s">
-        <v>2</v>
+        <v>239</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>928</v>
+        <v>706</v>
       </c>
       <c r="B189" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C189" t="s">
-        <v>204</v>
+        <v>83</v>
       </c>
       <c r="D189" t="s">
         <v>2</v>
@@ -3881,13 +3896,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>927</v>
+        <v>730</v>
       </c>
       <c r="B190" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C190" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="D190" t="s">
         <v>2</v>
@@ -3895,111 +3910,111 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>96</v>
+        <v>900</v>
       </c>
       <c r="B191" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C191" t="s">
-        <v>206</v>
+        <v>3</v>
       </c>
       <c r="D191" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>97</v>
+        <v>901</v>
       </c>
       <c r="B192" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="C192" t="s">
-        <v>207</v>
+        <v>66</v>
       </c>
       <c r="D192" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>98</v>
+        <v>902</v>
       </c>
       <c r="B193" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="C193" t="s">
-        <v>208</v>
+        <v>67</v>
       </c>
       <c r="D193" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>79</v>
+        <v>903</v>
       </c>
       <c r="B194" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="C194" t="s">
-        <v>209</v>
+        <v>47</v>
       </c>
       <c r="D194" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>78</v>
+        <v>904</v>
       </c>
       <c r="B195" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="C195" t="s">
-        <v>210</v>
+        <v>62</v>
       </c>
       <c r="D195" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>77</v>
+        <v>905</v>
       </c>
       <c r="B196" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C196" t="s">
-        <v>211</v>
+        <v>63</v>
       </c>
       <c r="D196" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>76</v>
+        <v>906</v>
       </c>
       <c r="B197" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C197" t="s">
-        <v>212</v>
+        <v>68</v>
       </c>
       <c r="D197" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>75</v>
+        <v>927</v>
       </c>
       <c r="B198" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C198" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D198" t="s">
         <v>2</v>
@@ -4007,13 +4022,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>74</v>
+        <v>928</v>
       </c>
       <c r="B199" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C199" t="s">
-        <v>130</v>
+        <v>204</v>
       </c>
       <c r="D199" t="s">
         <v>2</v>
@@ -4021,13 +4036,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>73</v>
+        <v>929</v>
       </c>
       <c r="B200" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C200" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="D200" t="s">
         <v>2</v>
@@ -4035,13 +4050,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>72</v>
+        <v>930</v>
       </c>
       <c r="B201" t="s">
         <v>54</v>
       </c>
       <c r="C201" t="s">
-        <v>215</v>
+        <v>136</v>
       </c>
       <c r="D201" t="s">
         <v>2</v>
@@ -4049,13 +4064,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>71</v>
+        <v>931</v>
       </c>
       <c r="B202" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C202" t="s">
-        <v>216</v>
+        <v>133</v>
       </c>
       <c r="D202" t="s">
         <v>2</v>
@@ -4063,13 +4078,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>70</v>
+        <v>932</v>
       </c>
       <c r="B203" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="C203" t="s">
-        <v>217</v>
+        <v>132</v>
       </c>
       <c r="D203" t="s">
         <v>2</v>
@@ -4077,13 +4092,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>506</v>
+        <v>933</v>
       </c>
       <c r="B204" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
       <c r="C204" t="s">
-        <v>219</v>
+        <v>131</v>
       </c>
       <c r="D204" t="s">
         <v>2</v>
@@ -4091,13 +4106,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>69</v>
+        <v>934</v>
       </c>
       <c r="B205" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="C205" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="D205" t="s">
         <v>2</v>
@@ -4105,13 +4120,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>68</v>
+        <v>935</v>
       </c>
       <c r="B206" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="C206" t="s">
-        <v>221</v>
+        <v>129</v>
       </c>
       <c r="D206" t="s">
         <v>2</v>
@@ -4119,13 +4134,13 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>67</v>
+        <v>936</v>
       </c>
       <c r="B207" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="C207" t="s">
-        <v>222</v>
+        <v>87</v>
       </c>
       <c r="D207" t="s">
         <v>2</v>
@@ -4133,13 +4148,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>66</v>
+        <v>937</v>
       </c>
       <c r="B208" t="s">
-        <v>223</v>
-      </c>
-      <c r="C208" t="s">
-        <v>224</v>
+        <v>86</v>
       </c>
       <c r="D208" t="s">
         <v>2</v>
@@ -4147,13 +4159,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>65</v>
+        <v>938</v>
       </c>
       <c r="B209" t="s">
-        <v>69</v>
-      </c>
-      <c r="C209" t="s">
-        <v>225</v>
+        <v>86</v>
       </c>
       <c r="D209" t="s">
         <v>2</v>
@@ -4161,13 +4170,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>64</v>
+        <v>939</v>
       </c>
       <c r="B210" t="s">
-        <v>46</v>
-      </c>
-      <c r="C210" t="s">
-        <v>226</v>
+        <v>86</v>
       </c>
       <c r="D210" t="s">
         <v>2</v>
@@ -4175,13 +4181,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>63</v>
+        <v>940</v>
       </c>
       <c r="B211" t="s">
-        <v>46</v>
-      </c>
-      <c r="C211" t="s">
-        <v>227</v>
+        <v>86</v>
       </c>
       <c r="D211" t="s">
         <v>2</v>
@@ -4189,13 +4192,13 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>62</v>
+        <v>941</v>
       </c>
       <c r="B212" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C212" t="s">
-        <v>228</v>
+        <v>88</v>
       </c>
       <c r="D212" t="s">
         <v>2</v>
@@ -4203,13 +4206,13 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>61</v>
+        <v>960</v>
       </c>
       <c r="B213" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C213" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="D213" t="s">
         <v>2</v>
@@ -4217,13 +4220,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>60</v>
+        <v>961</v>
       </c>
       <c r="B214" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C214" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="D214" t="s">
         <v>2</v>
@@ -4231,13 +4234,13 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>59</v>
+        <v>962</v>
       </c>
       <c r="B215" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C215" t="s">
-        <v>231</v>
+        <v>89</v>
       </c>
       <c r="D215" t="s">
         <v>2</v>
@@ -4245,13 +4248,13 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>58</v>
+        <v>963</v>
       </c>
       <c r="B216" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C216" t="s">
-        <v>232</v>
+        <v>90</v>
       </c>
       <c r="D216" t="s">
         <v>2</v>
@@ -4259,13 +4262,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>57</v>
+        <v>964</v>
       </c>
       <c r="B217" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C217" t="s">
-        <v>233</v>
+        <v>91</v>
       </c>
       <c r="D217" t="s">
         <v>2</v>
@@ -4273,13 +4276,13 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>56</v>
+        <v>965</v>
       </c>
       <c r="B218" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="C218" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="D218" t="s">
         <v>2</v>
@@ -4287,13 +4290,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>55</v>
+        <v>966</v>
       </c>
       <c r="B219" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="C219" t="s">
-        <v>235</v>
+        <v>141</v>
       </c>
       <c r="D219" t="s">
         <v>2</v>
@@ -4301,69 +4304,69 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220">
+        <v>967</v>
+      </c>
+      <c r="B220" t="s">
         <v>54</v>
       </c>
-      <c r="B220" t="s">
-        <v>194</v>
-      </c>
       <c r="C220" t="s">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="D220" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>53</v>
+        <v>968</v>
       </c>
       <c r="B221" t="s">
-        <v>194</v>
+        <v>54</v>
       </c>
       <c r="C221" t="s">
-        <v>236</v>
+        <v>93</v>
       </c>
       <c r="D221" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>52</v>
+        <v>969</v>
       </c>
       <c r="B222" t="s">
-        <v>194</v>
+        <v>54</v>
       </c>
       <c r="C222" t="s">
-        <v>237</v>
+        <v>94</v>
       </c>
       <c r="D222" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>51</v>
+        <v>970</v>
       </c>
       <c r="B223" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C223" t="s">
-        <v>240</v>
+        <v>95</v>
       </c>
       <c r="D223" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>50</v>
+        <v>971</v>
       </c>
       <c r="B224" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C224" t="s">
-        <v>241</v>
+        <v>97</v>
       </c>
       <c r="D224" t="s">
         <v>2</v>
@@ -4371,13 +4374,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>49</v>
+        <v>972</v>
       </c>
       <c r="B225" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C225" t="s">
-        <v>242</v>
+        <v>96</v>
       </c>
       <c r="D225" t="s">
         <v>2</v>
@@ -4385,13 +4388,13 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>48</v>
+        <v>973</v>
       </c>
       <c r="B226" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C226" t="s">
-        <v>243</v>
+        <v>98</v>
       </c>
       <c r="D226" t="s">
         <v>2</v>
@@ -4399,13 +4402,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>47</v>
+        <v>974</v>
       </c>
       <c r="B227" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C227" t="s">
-        <v>244</v>
+        <v>99</v>
       </c>
       <c r="D227" t="s">
         <v>2</v>
@@ -4413,13 +4416,13 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>46</v>
+        <v>975</v>
       </c>
       <c r="B228" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C228" t="s">
-        <v>245</v>
+        <v>100</v>
       </c>
       <c r="D228" t="s">
         <v>2</v>
@@ -4427,13 +4430,13 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>45</v>
+        <v>976</v>
       </c>
       <c r="B229" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C229" t="s">
-        <v>246</v>
+        <v>101</v>
       </c>
       <c r="D229" t="s">
         <v>2</v>
@@ -4441,13 +4444,13 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>44</v>
+        <v>977</v>
       </c>
       <c r="B230" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C230" t="s">
-        <v>247</v>
+        <v>102</v>
       </c>
       <c r="D230" t="s">
         <v>2</v>
@@ -4455,13 +4458,13 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>43</v>
+        <v>978</v>
       </c>
       <c r="B231" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C231" t="s">
-        <v>248</v>
+        <v>103</v>
       </c>
       <c r="D231" t="s">
         <v>2</v>
@@ -4469,13 +4472,13 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>42</v>
+        <v>979</v>
       </c>
       <c r="B232" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="C232" t="s">
-        <v>249</v>
+        <v>104</v>
       </c>
       <c r="D232" t="s">
         <v>2</v>
@@ -4483,13 +4486,13 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>41</v>
+        <v>980</v>
       </c>
       <c r="B233" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C233" t="s">
-        <v>250</v>
+        <v>105</v>
       </c>
       <c r="D233" t="s">
         <v>2</v>
@@ -4497,13 +4500,13 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>40</v>
+        <v>981</v>
       </c>
       <c r="B234" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C234" t="s">
-        <v>251</v>
+        <v>107</v>
       </c>
       <c r="D234" t="s">
         <v>2</v>
@@ -4511,13 +4514,13 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>39</v>
+        <v>982</v>
       </c>
       <c r="B235" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C235" t="s">
-        <v>252</v>
+        <v>109</v>
       </c>
       <c r="D235" t="s">
         <v>2</v>
@@ -4525,13 +4528,13 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>38</v>
+        <v>983</v>
       </c>
       <c r="B236" t="s">
-        <v>255</v>
+        <v>108</v>
       </c>
       <c r="C236" t="s">
-        <v>256</v>
+        <v>110</v>
       </c>
       <c r="D236" t="s">
         <v>2</v>
@@ -4539,13 +4542,13 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>37</v>
+        <v>984</v>
       </c>
       <c r="B237" t="s">
-        <v>255</v>
+        <v>108</v>
       </c>
       <c r="C237" t="s">
-        <v>257</v>
+        <v>111</v>
       </c>
       <c r="D237" t="s">
         <v>2</v>
@@ -4553,13 +4556,13 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>36</v>
+        <v>985</v>
       </c>
       <c r="B238" t="s">
-        <v>255</v>
+        <v>108</v>
       </c>
       <c r="C238" t="s">
-        <v>258</v>
+        <v>112</v>
       </c>
       <c r="D238" t="s">
         <v>2</v>
@@ -4567,13 +4570,13 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>35</v>
+        <v>986</v>
       </c>
       <c r="B239" t="s">
-        <v>259</v>
+        <v>108</v>
       </c>
       <c r="C239" t="s">
-        <v>260</v>
+        <v>113</v>
       </c>
       <c r="D239" t="s">
         <v>2</v>
@@ -4581,13 +4584,13 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>34</v>
+        <v>987</v>
       </c>
       <c r="B240" t="s">
-        <v>259</v>
+        <v>108</v>
       </c>
       <c r="C240" t="s">
-        <v>261</v>
+        <v>114</v>
       </c>
       <c r="D240" t="s">
         <v>2</v>
@@ -4595,13 +4598,13 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>33</v>
+        <v>988</v>
       </c>
       <c r="B241" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="C241" t="s">
-        <v>262</v>
+        <v>115</v>
       </c>
       <c r="D241" t="s">
         <v>2</v>
@@ -4609,13 +4612,13 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>32</v>
+        <v>989</v>
       </c>
       <c r="B242" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="C242" t="s">
-        <v>263</v>
+        <v>116</v>
       </c>
       <c r="D242" t="s">
         <v>2</v>
@@ -4623,13 +4626,13 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>31</v>
+        <v>990</v>
       </c>
       <c r="B243" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="C243" t="s">
-        <v>264</v>
+        <v>117</v>
       </c>
       <c r="D243" t="s">
         <v>2</v>
@@ -4637,13 +4640,13 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>30</v>
+        <v>991</v>
       </c>
       <c r="B244" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="C244" t="s">
-        <v>268</v>
+        <v>118</v>
       </c>
       <c r="D244" t="s">
         <v>2</v>
@@ -4651,13 +4654,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>29</v>
+        <v>992</v>
       </c>
       <c r="B245" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="C245" t="s">
-        <v>265</v>
+        <v>119</v>
       </c>
       <c r="D245" t="s">
         <v>2</v>
@@ -4665,13 +4668,13 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>28</v>
+        <v>993</v>
       </c>
       <c r="B246" t="s">
-        <v>259</v>
+        <v>120</v>
       </c>
       <c r="C246" t="s">
-        <v>266</v>
+        <v>121</v>
       </c>
       <c r="D246" t="s">
         <v>2</v>
@@ -4679,13 +4682,13 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>27</v>
+        <v>994</v>
       </c>
       <c r="B247" t="s">
-        <v>259</v>
+        <v>54</v>
       </c>
       <c r="C247" t="s">
-        <v>267</v>
+        <v>122</v>
       </c>
       <c r="D247" t="s">
         <v>2</v>
@@ -4693,13 +4696,13 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>26</v>
+        <v>995</v>
       </c>
       <c r="B248" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C248" t="s">
-        <v>269</v>
+        <v>124</v>
       </c>
       <c r="D248" t="s">
         <v>2</v>
@@ -4707,13 +4710,13 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249">
-        <v>25</v>
+        <v>996</v>
       </c>
       <c r="B249" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="C249" t="s">
-        <v>270</v>
+        <v>125</v>
       </c>
       <c r="D249" t="s">
         <v>2</v>
@@ -4721,13 +4724,13 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>24</v>
+        <v>997</v>
       </c>
       <c r="B250" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C250" t="s">
-        <v>271</v>
+        <v>126</v>
       </c>
       <c r="D250" t="s">
         <v>2</v>
@@ -4735,13 +4738,13 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>23</v>
+        <v>998</v>
       </c>
       <c r="B251" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="C251" t="s">
-        <v>272</v>
+        <v>127</v>
       </c>
       <c r="D251" t="s">
         <v>2</v>
@@ -4749,35 +4752,49 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>22</v>
+        <v>999</v>
       </c>
       <c r="B252" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="C252" t="s">
-        <v>273</v>
+        <v>128</v>
       </c>
       <c r="D252" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253">
-        <v>21</v>
+      <c r="A253" t="s">
+        <v>51</v>
       </c>
       <c r="B253" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="C253" t="s">
-        <v>274</v>
+        <v>53</v>
       </c>
       <c r="D253" t="s">
-        <v>2</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>1000</v>
+      </c>
+      <c r="B254" t="s">
+        <v>123</v>
+      </c>
+      <c r="C254" t="s">
+        <v>275</v>
+      </c>
+      <c r="D254" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2">
-    <sortState ref="A3:D173">
+    <sortState ref="A3:D253">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Put panthomjs screenshot back to the program.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="277">
   <si>
     <t>Number</t>
   </si>
@@ -855,6 +855,9 @@
   </si>
   <si>
     <t>Not a valid image format.</t>
+  </si>
+  <si>
+    <t>Parent information has been updated.</t>
   </si>
 </sst>
 </file>
@@ -1241,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H254"/>
+  <dimension ref="A1:H255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="C247" sqref="C247"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4790,6 +4793,17 @@
       </c>
       <c r="D254" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>20</v>
+      </c>
+      <c r="B255" t="s">
+        <v>106</v>
+      </c>
+      <c r="C255" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add (Private) tag right next to tree name / Remove dropdown box for Alive or Dead -> Red execute button (only for manager).
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="280">
   <si>
     <t>Number</t>
   </si>
@@ -858,6 +858,15 @@
   </si>
   <si>
     <t>Parent information has been updated.</t>
+  </si>
+  <si>
+    <t>THIS TREE IS DEAD</t>
+  </si>
+  <si>
+    <t>Press the button to set this tree as dead.</t>
+  </si>
+  <si>
+    <t>DEAD</t>
   </si>
 </sst>
 </file>
@@ -1244,9 +1253,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H255"/>
+  <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
       <selection activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
@@ -4804,6 +4813,51 @@
       </c>
       <c r="C255" t="s">
         <v>276</v>
+      </c>
+      <c r="D255" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>1001</v>
+      </c>
+      <c r="B256" t="s">
+        <v>69</v>
+      </c>
+      <c r="C256" t="s">
+        <v>277</v>
+      </c>
+      <c r="D256" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>1002</v>
+      </c>
+      <c r="B257" t="s">
+        <v>69</v>
+      </c>
+      <c r="C257" t="s">
+        <v>278</v>
+      </c>
+      <c r="D257" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>1003</v>
+      </c>
+      <c r="B258" t="s">
+        <v>69</v>
+      </c>
+      <c r="C258" t="s">
+        <v>279</v>
+      </c>
+      <c r="D258" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add manager password change.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="281">
   <si>
     <t>Number</t>
   </si>
@@ -867,6 +867,9 @@
   </si>
   <si>
     <t>DEAD</t>
+  </si>
+  <si>
+    <t>Confirm the password…</t>
   </si>
 </sst>
 </file>
@@ -1253,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H258"/>
+  <dimension ref="A1:H259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="C258" sqref="C258"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="C257" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4857,6 +4860,20 @@
         <v>279</v>
       </c>
       <c r="D258" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>1004</v>
+      </c>
+      <c r="B259" t="s">
+        <v>106</v>
+      </c>
+      <c r="C259" t="s">
+        <v>280</v>
+      </c>
+      <c r="D259" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add parent activities tab.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="288">
   <si>
     <t>Number</t>
   </si>
@@ -870,6 +870,27 @@
   </si>
   <si>
     <t>Confirm the password…</t>
+  </si>
+  <si>
+    <t>Password doesn't match.</t>
+  </si>
+  <si>
+    <t>Password has to be longer than 5 characters.</t>
+  </si>
+  <si>
+    <t>PARENT ACTIVITIES</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>contribution(s)</t>
+  </si>
+  <si>
+    <t>since</t>
+  </si>
+  <si>
+    <t>Recent 10 Posts</t>
   </si>
 </sst>
 </file>
@@ -1256,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H259"/>
+  <dimension ref="A1:H266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="C266" sqref="C266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,6 +4895,104 @@
         <v>280</v>
       </c>
       <c r="D259" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>1005</v>
+      </c>
+      <c r="B260" t="s">
+        <v>106</v>
+      </c>
+      <c r="C260" t="s">
+        <v>281</v>
+      </c>
+      <c r="D260" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>1006</v>
+      </c>
+      <c r="B261" t="s">
+        <v>106</v>
+      </c>
+      <c r="C261" t="s">
+        <v>282</v>
+      </c>
+      <c r="D261" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>1007</v>
+      </c>
+      <c r="B262" t="s">
+        <v>106</v>
+      </c>
+      <c r="C262" t="s">
+        <v>283</v>
+      </c>
+      <c r="D262" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>1008</v>
+      </c>
+      <c r="B263" t="s">
+        <v>106</v>
+      </c>
+      <c r="C263" t="s">
+        <v>285</v>
+      </c>
+      <c r="D263" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>1009</v>
+      </c>
+      <c r="B264" t="s">
+        <v>106</v>
+      </c>
+      <c r="C264" t="s">
+        <v>284</v>
+      </c>
+      <c r="D264" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>1010</v>
+      </c>
+      <c r="B265" t="s">
+        <v>106</v>
+      </c>
+      <c r="C265" t="s">
+        <v>286</v>
+      </c>
+      <c r="D265" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>1011</v>
+      </c>
+      <c r="B266" t="s">
+        <v>106</v>
+      </c>
+      <c r="C266" t="s">
+        <v>287</v>
+      </c>
+      <c r="D266" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Show adopted tree by parent on parent activiries panel.
</commit_message>
<xml_diff>
--- a/serverconfig/errorlist.xlsx
+++ b/serverconfig/errorlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="292">
   <si>
     <t>Number</t>
   </si>
@@ -891,6 +891,18 @@
   </si>
   <si>
     <t>Recent 10 Posts</t>
+  </si>
+  <si>
+    <t>No trees are under your watch.</t>
+  </si>
+  <si>
+    <t>tree(s) is/are currently adopted by you.</t>
+  </si>
+  <si>
+    <t>Season Trees</t>
+  </si>
+  <si>
+    <t>Non-season Trees</t>
   </si>
 </sst>
 </file>
@@ -1277,10 +1289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H266"/>
+  <dimension ref="A1:H270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
-      <selection activeCell="C266" sqref="C266"/>
+    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="C270" sqref="C270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,6 +5005,62 @@
         <v>287</v>
       </c>
       <c r="D266" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>1012</v>
+      </c>
+      <c r="B267" t="s">
+        <v>106</v>
+      </c>
+      <c r="C267" t="s">
+        <v>289</v>
+      </c>
+      <c r="D267" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>1013</v>
+      </c>
+      <c r="B268" t="s">
+        <v>106</v>
+      </c>
+      <c r="C268" t="s">
+        <v>288</v>
+      </c>
+      <c r="D268" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>1014</v>
+      </c>
+      <c r="B269" t="s">
+        <v>106</v>
+      </c>
+      <c r="C269" t="s">
+        <v>290</v>
+      </c>
+      <c r="D269" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>1015</v>
+      </c>
+      <c r="B270" t="s">
+        <v>106</v>
+      </c>
+      <c r="C270" t="s">
+        <v>291</v>
+      </c>
+      <c r="D270" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>